<commit_message>
#10445 - Adiciona novos testes e adiciona enviode email
</commit_message>
<xml_diff>
--- a/src/test/resources/arquivo_usuario/planilha.xlsx
+++ b/src/test/resources/arquivo_usuario/planilha.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="49">
   <si>
     <t xml:space="preserve">NIVEL/CANAL</t>
   </si>
@@ -140,109 +140,7 @@
     <t xml:space="preserve">ANALICE DA CONCEICAO</t>
   </si>
   <si>
-    <t xml:space="preserve">n.analice.conceicao@aec.com.br</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ANDERSON MATHEUS BALBINO DA SILVA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">n.anderson.bsilva@aec.com.br</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ANDREIA VIDAL DE NEGREIROS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">n.andreia.negreiros@aec.com.br</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ANDREZA DOS SANTOS RAMOS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">n.andreza.ramos@aec.com.br</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ANDREZZA PEREIRA DE LUCENA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">n.andrezza.lucena@aec.com.br</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ARETUZA NOGUEIRA DE LIMA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">n.aretuza.lima@aec.com.br</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ARTHUR ITALO SILVA SANTOS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">n.arthur.ssantos@aec.com.br</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ARTHUR WENDELL SOBREIRA DE BRITO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">n.arthur.brito@aec.com.br</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AYSLANIA COSTA E SILVA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">n.ayslania.silva@aec.com.br</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BRENDA CRISTIAN SOARES DE SOUSA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">n.brenda.sousa@aec.com.br</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BRUNA MICKAELLY ALVES DE BRITO MATEUS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">n.bruna.mateus@aec.com.br</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CALLYSON EMANUEL BALBINO DINIZ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">n.callyson.diniz@aec.com.br</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CAMILA LACERDA SANTOS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">n.camila.santos@aec.com.br</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CARLOS ALBERTO FELIPE OLIMPIO COSME DE LIMA GUERRA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">n.carlos.guerra@aec.com.br</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CATARINA COSTA BORJA RAMALHO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">n.catarina.ramalho@aec.com.br</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CHRISTIAN VIRGINIO ANDRADE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">n.christian.andrade@aec.com.br</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DAMARES BATISTA DE SOUZA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">n.damares.souza@aec.com.br</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DANIEL GERMANO DE ARAUJO FILHO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">n.daniel.filho@aec.com.br</t>
+    <t xml:space="preserve">n.analice.conceica.com.br</t>
   </si>
   <si>
     <t xml:space="preserve">AGENTE AUTORIZADO NACIONAL</t>
@@ -463,69 +361,27 @@
     <cellStyle name="*unknown*" xfId="20" builtinId="8" customBuiltin="false"/>
   </cellStyles>
   <dxfs count="21">
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
+    <dxf/>
+    <dxf/>
+    <dxf/>
+    <dxf/>
+    <dxf/>
+    <dxf/>
+    <dxf/>
+    <dxf/>
+    <dxf/>
+    <dxf/>
+    <dxf/>
+    <dxf/>
+    <dxf/>
+    <dxf/>
+    <dxf/>
+    <dxf/>
+    <dxf/>
+    <dxf/>
+    <dxf/>
+    <dxf/>
+    <dxf/>
   </dxfs>
   <colors>
     <indexedColors>
@@ -537,7 +393,7 @@
       <rgbColor rgb="FFFFFF00"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF9C0006"/>
+      <rgbColor rgb="FF800000"/>
       <rgbColor rgb="FF008000"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FF808000"/>
@@ -568,7 +424,7 @@
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFC7CE"/>
+      <rgbColor rgb="FFFFCC99"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
@@ -597,23 +453,23 @@
   </sheetPr>
   <dimension ref="1:44"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D26" activeCellId="0" sqref="D26"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E21" activeCellId="0" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.95"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="48.7295918367347"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="33.2091836734694"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="22.0051020408163"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="18.2244897959184"/>
-    <col collapsed="false" hidden="false" max="13" min="8" style="2" width="7.96428571428571"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="2" width="20.3826530612245"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="2" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="16" style="2" width="7.96428571428571"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="47.515306122449"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="32.265306122449"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="21.4642857142857"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="13" min="8" style="2" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="2" width="19.8418367346939"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="2" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="16" style="2" width="7.69387755102041"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2706,9 +2562,7 @@
       <c r="C3" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="11" t="n">
-        <v>6775206461</v>
-      </c>
+      <c r="D3" s="11"/>
       <c r="E3" s="12" t="s">
         <v>12</v>
       </c>
@@ -15187,7 +15041,7 @@
         <v>35</v>
       </c>
       <c r="D15" s="11" t="n">
-        <v>5410434471</v>
+        <v>2131</v>
       </c>
       <c r="E15" s="12" t="s">
         <v>36</v>
@@ -17257,27 +17111,13 @@
       <c r="AMJ16" s="0"/>
     </row>
     <row r="17" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="D17" s="11" t="n">
-        <v>10736815481</v>
-      </c>
-      <c r="E17" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="F17" s="13" t="n">
-        <v>34898</v>
-      </c>
-      <c r="G17" s="7" t="n">
-        <v>51991301817</v>
-      </c>
+      <c r="A17" s="6"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="7"/>
       <c r="H17" s="0"/>
       <c r="I17" s="0"/>
       <c r="J17" s="0"/>
@@ -18297,27 +18137,13 @@
       <c r="AMJ17" s="0"/>
     </row>
     <row r="18" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="D18" s="11" t="n">
-        <v>70141197455</v>
-      </c>
-      <c r="E18" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="F18" s="13" t="n">
-        <v>35254</v>
-      </c>
-      <c r="G18" s="7" t="n">
-        <v>51991301817</v>
-      </c>
+      <c r="A18" s="6"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="7"/>
       <c r="H18" s="0"/>
       <c r="I18" s="0"/>
       <c r="J18" s="0"/>
@@ -19337,27 +19163,13 @@
       <c r="AMJ18" s="0"/>
     </row>
     <row r="19" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="D19" s="11" t="n">
-        <v>12503486410</v>
-      </c>
-      <c r="E19" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="F19" s="13" t="n">
-        <v>35205</v>
-      </c>
-      <c r="G19" s="7" t="n">
-        <v>51991301817</v>
-      </c>
+      <c r="A19" s="6"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="7"/>
       <c r="H19" s="0"/>
       <c r="I19" s="0"/>
       <c r="J19" s="0"/>
@@ -20377,27 +20189,13 @@
       <c r="AMJ19" s="0"/>
     </row>
     <row r="20" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="D20" s="11" t="n">
-        <v>4280058458</v>
-      </c>
-      <c r="E20" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="F20" s="13" t="n">
-        <v>29390</v>
-      </c>
-      <c r="G20" s="7" t="n">
-        <v>51991301817</v>
-      </c>
+      <c r="A20" s="6"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="7"/>
       <c r="H20" s="0"/>
       <c r="I20" s="0"/>
       <c r="J20" s="0"/>
@@ -21417,27 +21215,13 @@
       <c r="AMJ20" s="0"/>
     </row>
     <row r="21" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="D21" s="11" t="n">
-        <v>6185133458</v>
-      </c>
-      <c r="E21" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="F21" s="13" t="n">
-        <v>31124</v>
-      </c>
-      <c r="G21" s="7" t="n">
-        <v>51991301817</v>
-      </c>
+      <c r="A21" s="6"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="7"/>
       <c r="H21" s="0"/>
       <c r="I21" s="0"/>
       <c r="J21" s="0"/>
@@ -22457,27 +22241,13 @@
       <c r="AMJ21" s="0"/>
     </row>
     <row r="22" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="D22" s="11" t="n">
-        <v>9270740447</v>
-      </c>
-      <c r="E22" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="F22" s="13" t="n">
-        <v>33590</v>
-      </c>
-      <c r="G22" s="7" t="n">
-        <v>51991301817</v>
-      </c>
+      <c r="A22" s="6"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="7"/>
       <c r="H22" s="0"/>
       <c r="I22" s="0"/>
       <c r="J22" s="0"/>
@@ -23497,27 +23267,13 @@
       <c r="AMJ22" s="0"/>
     </row>
     <row r="23" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="D23" s="11" t="n">
-        <v>10025796437</v>
-      </c>
-      <c r="E23" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="F23" s="13" t="n">
-        <v>33716</v>
-      </c>
-      <c r="G23" s="7" t="n">
-        <v>51991301817</v>
-      </c>
+      <c r="A23" s="6"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="7"/>
       <c r="H23" s="0"/>
       <c r="I23" s="0"/>
       <c r="J23" s="0"/>
@@ -24537,27 +24293,13 @@
       <c r="AMJ23" s="0"/>
     </row>
     <row r="24" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="D24" s="11" t="n">
-        <v>10683287460</v>
-      </c>
-      <c r="E24" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="F24" s="13" t="n">
-        <v>34591</v>
-      </c>
-      <c r="G24" s="7" t="n">
-        <v>51991301817</v>
-      </c>
+      <c r="A24" s="6"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="7"/>
       <c r="H24" s="0"/>
       <c r="I24" s="0"/>
       <c r="J24" s="0"/>
@@ -25577,27 +25319,13 @@
       <c r="AMJ24" s="0"/>
     </row>
     <row r="25" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B25" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C25" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="D25" s="11" t="n">
-        <v>10887160409</v>
-      </c>
-      <c r="E25" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="F25" s="13" t="n">
-        <v>34176</v>
-      </c>
-      <c r="G25" s="7" t="n">
-        <v>51991301817</v>
-      </c>
+      <c r="A25" s="6"/>
+      <c r="B25" s="6"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="7"/>
       <c r="H25" s="0"/>
       <c r="I25" s="0"/>
       <c r="J25" s="0"/>
@@ -26617,27 +26345,13 @@
       <c r="AMJ25" s="0"/>
     </row>
     <row r="26" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B26" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C26" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="D26" s="11" t="n">
-        <v>70033392420</v>
-      </c>
-      <c r="E26" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="F26" s="13" t="n">
-        <v>34627</v>
-      </c>
-      <c r="G26" s="7" t="n">
-        <v>51991301817</v>
-      </c>
+      <c r="A26" s="6"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="13"/>
+      <c r="G26" s="7"/>
       <c r="H26" s="0"/>
       <c r="I26" s="0"/>
       <c r="J26" s="0"/>
@@ -27657,27 +27371,13 @@
       <c r="AMJ26" s="0"/>
     </row>
     <row r="27" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B27" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="D27" s="11" t="n">
-        <v>13117909770</v>
-      </c>
-      <c r="E27" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="F27" s="13" t="n">
-        <v>35067</v>
-      </c>
-      <c r="G27" s="7" t="n">
-        <v>51991301817</v>
-      </c>
+      <c r="A27" s="6"/>
+      <c r="B27" s="6"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="11"/>
+      <c r="E27" s="12"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="7"/>
       <c r="H27" s="0"/>
       <c r="I27" s="0"/>
       <c r="J27" s="0"/>
@@ -28697,27 +28397,13 @@
       <c r="AMJ27" s="0"/>
     </row>
     <row r="28" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B28" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C28" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="D28" s="11" t="n">
-        <v>11645863433</v>
-      </c>
-      <c r="E28" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="F28" s="13" t="n">
-        <v>34535</v>
-      </c>
-      <c r="G28" s="7" t="n">
-        <v>51991301817</v>
-      </c>
+      <c r="A28" s="6"/>
+      <c r="B28" s="6"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="12"/>
+      <c r="F28" s="13"/>
+      <c r="G28" s="7"/>
       <c r="H28" s="0"/>
       <c r="I28" s="0"/>
       <c r="J28" s="0"/>
@@ -29737,27 +29423,13 @@
       <c r="AMJ28" s="0"/>
     </row>
     <row r="29" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B29" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C29" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="D29" s="11" t="n">
-        <v>8331792416</v>
-      </c>
-      <c r="E29" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="F29" s="13" t="n">
-        <v>35795</v>
-      </c>
-      <c r="G29" s="7" t="n">
-        <v>51991301817</v>
-      </c>
+      <c r="A29" s="6"/>
+      <c r="B29" s="6"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="11"/>
+      <c r="E29" s="12"/>
+      <c r="F29" s="13"/>
+      <c r="G29" s="7"/>
       <c r="H29" s="0"/>
       <c r="I29" s="0"/>
       <c r="J29" s="0"/>
@@ -30777,27 +30449,13 @@
       <c r="AMJ29" s="0"/>
     </row>
     <row r="30" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B30" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C30" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="D30" s="11" t="n">
-        <v>3770293436</v>
-      </c>
-      <c r="E30" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="F30" s="13" t="n">
-        <v>28811</v>
-      </c>
-      <c r="G30" s="7" t="n">
-        <v>51991301817</v>
-      </c>
+      <c r="A30" s="6"/>
+      <c r="B30" s="6"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="11"/>
+      <c r="E30" s="12"/>
+      <c r="F30" s="13"/>
+      <c r="G30" s="7"/>
       <c r="H30" s="0"/>
       <c r="I30" s="0"/>
       <c r="J30" s="0"/>
@@ -31817,27 +31475,13 @@
       <c r="AMJ30" s="0"/>
     </row>
     <row r="31" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B31" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C31" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="D31" s="11" t="n">
-        <v>9015902402</v>
-      </c>
-      <c r="E31" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="F31" s="13" t="n">
-        <v>32954</v>
-      </c>
-      <c r="G31" s="7" t="n">
-        <v>51991301817</v>
-      </c>
+      <c r="A31" s="6"/>
+      <c r="B31" s="6"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="11"/>
+      <c r="E31" s="12"/>
+      <c r="F31" s="13"/>
+      <c r="G31" s="7"/>
       <c r="H31" s="0"/>
       <c r="I31" s="0"/>
       <c r="J31" s="0"/>
@@ -32857,27 +32501,13 @@
       <c r="AMJ31" s="0"/>
     </row>
     <row r="32" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B32" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C32" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="D32" s="11" t="n">
-        <v>1551748436</v>
-      </c>
-      <c r="E32" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="F32" s="13" t="n">
-        <v>31843</v>
-      </c>
-      <c r="G32" s="7" t="n">
-        <v>51991301817</v>
-      </c>
+      <c r="A32" s="6"/>
+      <c r="B32" s="6"/>
+      <c r="C32" s="6"/>
+      <c r="D32" s="11"/>
+      <c r="E32" s="12"/>
+      <c r="F32" s="13"/>
+      <c r="G32" s="7"/>
       <c r="H32" s="0"/>
       <c r="I32" s="0"/>
       <c r="J32" s="0"/>
@@ -33897,27 +33527,13 @@
       <c r="AMJ32" s="0"/>
     </row>
     <row r="33" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B33" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C33" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="D33" s="11" t="n">
-        <v>32690523833</v>
-      </c>
-      <c r="E33" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="F33" s="13" t="n">
-        <v>30727</v>
-      </c>
-      <c r="G33" s="7" t="n">
-        <v>51991301817</v>
-      </c>
+      <c r="A33" s="6"/>
+      <c r="B33" s="6"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="11"/>
+      <c r="E33" s="12"/>
+      <c r="F33" s="13"/>
+      <c r="G33" s="7"/>
       <c r="H33" s="0"/>
       <c r="I33" s="0"/>
       <c r="J33" s="0"/>
@@ -34937,27 +34553,13 @@
       <c r="AMJ33" s="0"/>
     </row>
     <row r="34" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B34" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C34" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="D34" s="11" t="n">
-        <v>10025796437</v>
-      </c>
-      <c r="E34" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="F34" s="13" t="n">
-        <v>33716</v>
-      </c>
-      <c r="G34" s="7" t="n">
-        <v>51991301817</v>
-      </c>
+      <c r="A34" s="6"/>
+      <c r="B34" s="6"/>
+      <c r="C34" s="6"/>
+      <c r="D34" s="11"/>
+      <c r="E34" s="12"/>
+      <c r="F34" s="13"/>
+      <c r="G34" s="7"/>
       <c r="H34" s="0"/>
       <c r="I34" s="0"/>
       <c r="J34" s="0"/>
@@ -35977,27 +35579,13 @@
       <c r="AMJ34" s="0"/>
     </row>
     <row r="35" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B35" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C35" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="D35" s="11" t="n">
-        <v>10683287460</v>
-      </c>
-      <c r="E35" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="F35" s="13" t="n">
-        <v>34591</v>
-      </c>
-      <c r="G35" s="7" t="n">
-        <v>51991301817</v>
-      </c>
+      <c r="A35" s="6"/>
+      <c r="B35" s="6"/>
+      <c r="C35" s="6"/>
+      <c r="D35" s="11"/>
+      <c r="E35" s="12"/>
+      <c r="F35" s="13"/>
+      <c r="G35" s="7"/>
       <c r="H35" s="0"/>
       <c r="I35" s="0"/>
       <c r="J35" s="0"/>
@@ -37017,27 +36605,13 @@
       <c r="AMJ35" s="0"/>
     </row>
     <row r="36" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B36" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C36" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="D36" s="11" t="n">
-        <v>10887160409</v>
-      </c>
-      <c r="E36" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="F36" s="13" t="n">
-        <v>34176</v>
-      </c>
-      <c r="G36" s="7" t="n">
-        <v>51991301817</v>
-      </c>
+      <c r="A36" s="6"/>
+      <c r="B36" s="6"/>
+      <c r="C36" s="6"/>
+      <c r="D36" s="11"/>
+      <c r="E36" s="12"/>
+      <c r="F36" s="13"/>
+      <c r="G36" s="7"/>
       <c r="H36" s="0"/>
       <c r="I36" s="0"/>
       <c r="J36" s="0"/>
@@ -38057,27 +37631,13 @@
       <c r="AMJ36" s="0"/>
     </row>
     <row r="37" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B37" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C37" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="D37" s="11" t="n">
-        <v>70033392420</v>
-      </c>
-      <c r="E37" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="F37" s="13" t="n">
-        <v>34627</v>
-      </c>
-      <c r="G37" s="7" t="n">
-        <v>51991301817</v>
-      </c>
+      <c r="A37" s="6"/>
+      <c r="B37" s="6"/>
+      <c r="C37" s="6"/>
+      <c r="D37" s="11"/>
+      <c r="E37" s="12"/>
+      <c r="F37" s="13"/>
+      <c r="G37" s="7"/>
       <c r="H37" s="0"/>
       <c r="I37" s="0"/>
       <c r="J37" s="0"/>
@@ -39097,27 +38657,13 @@
       <c r="AMJ37" s="0"/>
     </row>
     <row r="38" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B38" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C38" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="D38" s="11" t="n">
-        <v>13117909770</v>
-      </c>
-      <c r="E38" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="F38" s="13" t="n">
-        <v>35067</v>
-      </c>
-      <c r="G38" s="7" t="n">
-        <v>51991301817</v>
-      </c>
+      <c r="A38" s="6"/>
+      <c r="B38" s="6"/>
+      <c r="C38" s="6"/>
+      <c r="D38" s="11"/>
+      <c r="E38" s="12"/>
+      <c r="F38" s="13"/>
+      <c r="G38" s="7"/>
       <c r="H38" s="0"/>
       <c r="I38" s="0"/>
       <c r="J38" s="0"/>
@@ -40137,27 +39683,13 @@
       <c r="AMJ38" s="0"/>
     </row>
     <row r="39" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B39" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C39" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="D39" s="11" t="n">
-        <v>11645863433</v>
-      </c>
-      <c r="E39" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="F39" s="13" t="n">
-        <v>34535</v>
-      </c>
-      <c r="G39" s="7" t="n">
-        <v>51991301817</v>
-      </c>
+      <c r="A39" s="6"/>
+      <c r="B39" s="6"/>
+      <c r="C39" s="6"/>
+      <c r="D39" s="11"/>
+      <c r="E39" s="12"/>
+      <c r="F39" s="13"/>
+      <c r="G39" s="7"/>
       <c r="H39" s="0"/>
       <c r="I39" s="0"/>
       <c r="J39" s="0"/>
@@ -41177,27 +40709,13 @@
       <c r="AMJ39" s="0"/>
     </row>
     <row r="40" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A40" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B40" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C40" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="D40" s="11" t="n">
-        <v>8331792416</v>
-      </c>
-      <c r="E40" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="F40" s="13" t="n">
-        <v>35795</v>
-      </c>
-      <c r="G40" s="7" t="n">
-        <v>51991301817</v>
-      </c>
+      <c r="A40" s="6"/>
+      <c r="B40" s="6"/>
+      <c r="C40" s="6"/>
+      <c r="D40" s="11"/>
+      <c r="E40" s="12"/>
+      <c r="F40" s="13"/>
+      <c r="G40" s="7"/>
       <c r="H40" s="0"/>
       <c r="I40" s="0"/>
       <c r="J40" s="0"/>
@@ -42217,27 +41735,13 @@
       <c r="AMJ40" s="0"/>
     </row>
     <row r="41" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A41" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B41" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C41" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="D41" s="11" t="n">
-        <v>3770293436</v>
-      </c>
-      <c r="E41" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="F41" s="13" t="n">
-        <v>28811</v>
-      </c>
-      <c r="G41" s="7" t="n">
-        <v>51991301817</v>
-      </c>
+      <c r="A41" s="6"/>
+      <c r="B41" s="6"/>
+      <c r="C41" s="6"/>
+      <c r="D41" s="11"/>
+      <c r="E41" s="12"/>
+      <c r="F41" s="13"/>
+      <c r="G41" s="7"/>
       <c r="H41" s="0"/>
       <c r="I41" s="0"/>
       <c r="J41" s="0"/>
@@ -43257,27 +42761,13 @@
       <c r="AMJ41" s="0"/>
     </row>
     <row r="42" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A42" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B42" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C42" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="D42" s="11" t="n">
-        <v>9015902402</v>
-      </c>
-      <c r="E42" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="F42" s="13" t="n">
-        <v>32954</v>
-      </c>
-      <c r="G42" s="7" t="n">
-        <v>51991301817</v>
-      </c>
+      <c r="A42" s="6"/>
+      <c r="B42" s="6"/>
+      <c r="C42" s="6"/>
+      <c r="D42" s="11"/>
+      <c r="E42" s="12"/>
+      <c r="F42" s="13"/>
+      <c r="G42" s="7"/>
       <c r="H42" s="0"/>
       <c r="I42" s="0"/>
       <c r="J42" s="0"/>
@@ -44297,27 +43787,13 @@
       <c r="AMJ42" s="0"/>
     </row>
     <row r="43" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A43" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B43" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C43" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="D43" s="11" t="n">
-        <v>1551748436</v>
-      </c>
-      <c r="E43" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="F43" s="13" t="n">
-        <v>31843</v>
-      </c>
-      <c r="G43" s="7" t="n">
-        <v>51991301817</v>
-      </c>
+      <c r="A43" s="6"/>
+      <c r="B43" s="6"/>
+      <c r="C43" s="6"/>
+      <c r="D43" s="11"/>
+      <c r="E43" s="12"/>
+      <c r="F43" s="13"/>
+      <c r="G43" s="7"/>
       <c r="H43" s="0"/>
       <c r="I43" s="0"/>
       <c r="J43" s="0"/>
@@ -45337,27 +44813,13 @@
       <c r="AMJ43" s="0"/>
     </row>
     <row r="44" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A44" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B44" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C44" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="D44" s="11" t="n">
-        <v>32690523833</v>
-      </c>
-      <c r="E44" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="F44" s="13" t="n">
-        <v>30727</v>
-      </c>
-      <c r="G44" s="7" t="n">
-        <v>51991301817</v>
-      </c>
+      <c r="A44" s="6"/>
+      <c r="B44" s="6"/>
+      <c r="C44" s="6"/>
+      <c r="D44" s="11"/>
+      <c r="E44" s="12"/>
+      <c r="F44" s="13"/>
+      <c r="G44" s="7"/>
       <c r="H44" s="0"/>
       <c r="I44" s="0"/>
       <c r="J44" s="0"/>
@@ -46504,16 +45966,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="8.10204081632653"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="33.4795918367347"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.10204081632653"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.9336734693878"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="32.530612244898"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D4" s="0" t="s">
-        <v>73</v>
+        <v>39</v>
       </c>
       <c r="F4" s="0" t="s">
         <v>8</v>
@@ -46521,35 +45983,35 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D5" s="0" t="s">
-        <v>74</v>
+        <v>40</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>75</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D6" s="0" t="s">
-        <v>76</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D7" s="0" t="s">
-        <v>77</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D8" s="0" t="s">
-        <v>78</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D9" s="0" t="s">
-        <v>79</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D10" s="0" t="s">
-        <v>80</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -46559,12 +46021,12 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D12" s="0" t="s">
-        <v>81</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D13" s="0" t="s">
-        <v>82</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
#10445 - Adiciona testes para importação dos usuários
</commit_message>
<xml_diff>
--- a/src/test/resources/arquivo_usuario/planilha.xlsx
+++ b/src/test/resources/arquivo_usuario/planilha.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="50">
   <si>
     <t xml:space="preserve">NIVEL/CANAL</t>
   </si>
@@ -63,6 +63,9 @@
   </si>
   <si>
     <t xml:space="preserve">n.adenildo.oliveira@aec.com.br</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RECEPTIVA</t>
   </si>
   <si>
     <t xml:space="preserve">ADRIANA DE LIMA BEZERRA</t>
@@ -454,22 +457,22 @@
   <dimension ref="1:44"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E21" activeCellId="0" sqref="E21"/>
+      <selection pane="topLeft" activeCell="F22" activeCellId="0" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.95"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="47.515306122449"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="32.265306122449"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="21.4642857142857"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="13" min="8" style="2" width="7.69387755102041"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="2" width="19.8418367346939"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="2" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="16" style="2" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="46.9795918367347"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="31.8571428571429"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="21.1938775510204"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="13" min="8" style="2" width="7.56122448979592"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="2" width="19.5714285714286"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="2" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="16" style="2" width="7.56122448979592"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3592,19 +3595,19 @@
     </row>
     <row r="4" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D4" s="11" t="n">
         <v>70159931479</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F4" s="13" t="n">
         <v>34436</v>
@@ -4638,13 +4641,13 @@
         <v>8</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D5" s="11" t="n">
         <v>2917600403</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F5" s="13" t="n">
         <v>27678</v>
@@ -5678,13 +5681,13 @@
         <v>8</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D6" s="11" t="n">
         <v>9249138431</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F6" s="13" t="n">
         <v>32373</v>
@@ -6718,13 +6721,13 @@
         <v>8</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D7" s="11" t="n">
         <v>12532343451</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F7" s="13" t="n">
         <v>35926</v>
@@ -7758,13 +7761,13 @@
         <v>8</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D8" s="11" t="n">
         <v>11523845465</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F8" s="13" t="n">
         <v>34705</v>
@@ -8798,13 +8801,13 @@
         <v>8</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D9" s="11" t="n">
         <v>1581072414</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F9" s="13" t="n">
         <v>32575</v>
@@ -9838,13 +9841,13 @@
         <v>8</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D10" s="11" t="n">
         <v>10161857400</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F10" s="13" t="n">
         <v>33127</v>
@@ -10878,13 +10881,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D11" s="11" t="n">
         <v>10144034727</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F11" s="13" t="n">
         <v>31722</v>
@@ -11918,13 +11921,13 @@
         <v>8</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D12" s="11" t="n">
         <v>5985368416</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F12" s="13" t="n">
         <v>31827</v>
@@ -12958,13 +12961,13 @@
         <v>8</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D13" s="11" t="n">
         <v>70028986474</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F13" s="13" t="n">
         <v>34532</v>
@@ -13998,13 +14001,13 @@
         <v>8</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D14" s="11" t="n">
         <v>6920673452</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F14" s="13" t="n">
         <v>31751</v>
@@ -15038,13 +15041,13 @@
         <v>8</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D15" s="11" t="n">
         <v>2131</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F15" s="13" t="n">
         <v>30749</v>
@@ -16078,13 +16081,13 @@
         <v>8</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D16" s="11" t="n">
         <v>9460873421</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F16" s="13" t="n">
         <v>34055</v>
@@ -45966,16 +45969,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="32.530612244898"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="32.1275510204082"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D4" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F4" s="0" t="s">
         <v>8</v>
@@ -45983,35 +45986,35 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D5" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D6" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D7" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D8" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D9" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D10" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -46021,12 +46024,12 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D12" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D13" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adiciona validação de nivel, do tamanho de nome e de email
</commit_message>
<xml_diff>
--- a/src/test/resources/arquivo_usuario/planilha.xlsx
+++ b/src/test/resources/arquivo_usuario/planilha.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="54">
   <si>
     <t xml:space="preserve">NIVEL/CANAL</t>
   </si>
@@ -63,6 +63,9 @@
   </si>
   <si>
     <t xml:space="preserve">n.adaide.santos@aec.com.br</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AGENTE AUTORIZADO</t>
   </si>
   <si>
     <t xml:space="preserve">COMERCIAL</t>
@@ -255,7 +258,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="2">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -268,20 +271,6 @@
       <right style="hair"/>
       <top style="hair"/>
       <bottom style="hair"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top/>
-      <bottom style="thin"/>
       <diagonal/>
     </border>
   </borders>
@@ -313,7 +302,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -326,52 +315,36 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="3" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -478,23 +451,23 @@
   <dimension ref="1:49"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
+      <selection pane="topLeft" activeCell="I7" activeCellId="0" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="18.6734693877551"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="45.8979591836735"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="31.0459183673469"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="20.5204081632653"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="14" min="9" style="2" width="7.29081632653061"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="2" width="19.0357142857143"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="2" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="1025" min="17" style="2" width="7.29081632653061"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="45.3571428571429"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="30.6428571428571"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="20.25"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="14" min="9" style="2" width="7.1530612244898"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="2" width="18.765306122449"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="2" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="1025" min="17" style="2" width="7.1530612244898"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1540,28 +1513,28 @@
       <c r="AMJ1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="9" t="n">
+      <c r="E2" s="7" t="n">
         <v>10604168403</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="11" t="n">
+      <c r="G2" s="9" t="n">
         <v>34218</v>
       </c>
-      <c r="H2" s="8" t="n">
+      <c r="H2" s="1" t="n">
         <v>51991301817</v>
       </c>
       <c r="I2" s="0"/>
@@ -2582,26 +2555,26 @@
       <c r="AMJ2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="6" t="s">
-        <v>8</v>
+      <c r="A3" s="1" t="s">
+        <v>13</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="12"/>
-      <c r="F3" s="13" t="s">
+      <c r="D3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="14" t="n">
+      <c r="E3" s="7"/>
+      <c r="F3" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="9" t="n">
         <v>31944</v>
       </c>
-      <c r="H3" s="8" t="n">
+      <c r="H3" s="1" t="n">
         <v>51991301817</v>
       </c>
       <c r="I3" s="0"/>
@@ -3622,28 +3595,28 @@
       <c r="AMJ3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="6" t="s">
-        <v>16</v>
+      <c r="A4" s="1" t="s">
+        <v>17</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
-      <c r="D4" s="6" t="s">
-        <v>17</v>
+      <c r="D4" s="1" t="s">
+        <v>18</v>
       </c>
-      <c r="E4" s="12" t="n">
+      <c r="E4" s="7" t="n">
         <v>70159931479</v>
       </c>
-      <c r="F4" s="13" t="s">
-        <v>18</v>
+      <c r="F4" s="8" t="s">
+        <v>19</v>
       </c>
-      <c r="G4" s="14" t="n">
+      <c r="G4" s="9" t="n">
         <v>34436</v>
       </c>
-      <c r="H4" s="8" t="n">
+      <c r="H4" s="1" t="n">
         <v>51991301817</v>
       </c>
       <c r="I4" s="0"/>
@@ -4664,28 +4637,28 @@
       <c r="AMJ4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
-      <c r="D5" s="6" t="s">
-        <v>19</v>
+      <c r="D5" s="1" t="s">
+        <v>20</v>
       </c>
-      <c r="E5" s="12" t="n">
+      <c r="E5" s="7" t="n">
         <v>2917600403</v>
       </c>
-      <c r="F5" s="13" t="s">
-        <v>20</v>
+      <c r="F5" s="8" t="s">
+        <v>21</v>
       </c>
-      <c r="G5" s="14" t="n">
+      <c r="G5" s="9" t="n">
         <v>27678</v>
       </c>
-      <c r="H5" s="8" t="n">
+      <c r="H5" s="1" t="n">
         <v>51991301817</v>
       </c>
       <c r="I5" s="0"/>
@@ -5706,28 +5679,28 @@
       <c r="AMJ5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
-      <c r="D6" s="6" t="s">
-        <v>21</v>
+      <c r="D6" s="1" t="s">
+        <v>22</v>
       </c>
-      <c r="E6" s="12" t="n">
+      <c r="E6" s="7" t="n">
         <v>9249138431</v>
       </c>
-      <c r="F6" s="13" t="s">
-        <v>22</v>
+      <c r="F6" s="8" t="s">
+        <v>23</v>
       </c>
-      <c r="G6" s="14" t="n">
+      <c r="G6" s="9" t="n">
         <v>32373</v>
       </c>
-      <c r="H6" s="8" t="n">
+      <c r="H6" s="1" t="n">
         <v>51991301817</v>
       </c>
       <c r="I6" s="0"/>
@@ -6748,28 +6721,28 @@
       <c r="AMJ6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
-      <c r="D7" s="6" t="s">
-        <v>23</v>
+      <c r="D7" s="1" t="s">
+        <v>24</v>
       </c>
-      <c r="E7" s="12" t="n">
+      <c r="E7" s="7" t="n">
         <v>12532343451</v>
       </c>
-      <c r="F7" s="13" t="s">
-        <v>24</v>
+      <c r="F7" s="8" t="s">
+        <v>25</v>
       </c>
-      <c r="G7" s="14" t="n">
+      <c r="G7" s="9" t="n">
         <v>35926</v>
       </c>
-      <c r="H7" s="8" t="n">
+      <c r="H7" s="1" t="n">
         <v>51991301817</v>
       </c>
       <c r="I7" s="0"/>
@@ -7790,28 +7763,28 @@
       <c r="AMJ7" s="0"/>
     </row>
     <row r="8" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
-      <c r="D8" s="6" t="s">
-        <v>25</v>
+      <c r="D8" s="1" t="s">
+        <v>26</v>
       </c>
-      <c r="E8" s="12" t="n">
+      <c r="E8" s="7" t="n">
         <v>11523845465</v>
       </c>
-      <c r="F8" s="13" t="s">
-        <v>26</v>
+      <c r="F8" s="8" t="s">
+        <v>27</v>
       </c>
-      <c r="G8" s="14" t="n">
+      <c r="G8" s="9" t="n">
         <v>34705</v>
       </c>
-      <c r="H8" s="8" t="n">
+      <c r="H8" s="1" t="n">
         <v>51991301817</v>
       </c>
       <c r="I8" s="0"/>
@@ -8832,28 +8805,28 @@
       <c r="AMJ8" s="0"/>
     </row>
     <row r="9" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
-      <c r="D9" s="6" t="s">
-        <v>27</v>
+      <c r="D9" s="1" t="s">
+        <v>28</v>
       </c>
-      <c r="E9" s="12" t="n">
+      <c r="E9" s="7" t="n">
         <v>1581072414</v>
       </c>
-      <c r="F9" s="13" t="s">
-        <v>28</v>
+      <c r="F9" s="8" t="s">
+        <v>29</v>
       </c>
-      <c r="G9" s="14" t="n">
+      <c r="G9" s="9" t="n">
         <v>32575</v>
       </c>
-      <c r="H9" s="8" t="n">
+      <c r="H9" s="1" t="n">
         <v>51991301817</v>
       </c>
       <c r="I9" s="0"/>
@@ -9874,28 +9847,28 @@
       <c r="AMJ9" s="0"/>
     </row>
     <row r="10" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
-      <c r="D10" s="6" t="s">
-        <v>29</v>
+      <c r="D10" s="1" t="s">
+        <v>30</v>
       </c>
-      <c r="E10" s="12" t="n">
+      <c r="E10" s="7" t="n">
         <v>10161857400</v>
       </c>
-      <c r="F10" s="13" t="s">
-        <v>30</v>
+      <c r="F10" s="8" t="s">
+        <v>31</v>
       </c>
-      <c r="G10" s="14" t="n">
+      <c r="G10" s="9" t="n">
         <v>33127</v>
       </c>
-      <c r="H10" s="8" t="n">
+      <c r="H10" s="1" t="n">
         <v>51991301817</v>
       </c>
       <c r="I10" s="0"/>
@@ -10916,13 +10889,10 @@
       <c r="AMJ10" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="6"/>
-      <c r="B11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="8"/>
+      <c r="C11" s="10"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="9"/>
       <c r="I11" s="0"/>
       <c r="J11" s="0"/>
       <c r="K11" s="0"/>
@@ -11941,13 +11911,10 @@
       <c r="AMJ11" s="0"/>
     </row>
     <row r="12" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="6"/>
-      <c r="B12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="8"/>
+      <c r="C12" s="10"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="9"/>
       <c r="I12" s="0"/>
       <c r="J12" s="0"/>
       <c r="K12" s="0"/>
@@ -12966,13 +12933,10 @@
       <c r="AMJ12" s="0"/>
     </row>
     <row r="13" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="6"/>
-      <c r="B13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="8"/>
+      <c r="C13" s="10"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="9"/>
       <c r="I13" s="0"/>
       <c r="J13" s="0"/>
       <c r="K13" s="0"/>
@@ -13991,13 +13955,10 @@
       <c r="AMJ13" s="0"/>
     </row>
     <row r="14" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="6"/>
-      <c r="B14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="8"/>
+      <c r="C14" s="10"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="9"/>
       <c r="I14" s="0"/>
       <c r="J14" s="0"/>
       <c r="K14" s="0"/>
@@ -15016,13 +14977,10 @@
       <c r="AMJ14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="6"/>
-      <c r="B15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="8"/>
+      <c r="C15" s="10"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="9"/>
       <c r="I15" s="0"/>
       <c r="J15" s="0"/>
       <c r="K15" s="0"/>
@@ -16041,28 +15999,28 @@
       <c r="AMJ15" s="0"/>
     </row>
     <row r="16" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="6" t="s">
+      <c r="A16" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
-      <c r="D16" s="6" t="s">
-        <v>31</v>
+      <c r="D16" s="1" t="s">
+        <v>32</v>
       </c>
-      <c r="E16" s="12" t="n">
+      <c r="E16" s="7" t="n">
         <v>10144034727</v>
       </c>
-      <c r="F16" s="13" t="s">
-        <v>32</v>
+      <c r="F16" s="8" t="s">
+        <v>33</v>
       </c>
-      <c r="G16" s="14" t="n">
+      <c r="G16" s="9" t="n">
         <v>31722</v>
       </c>
-      <c r="H16" s="8" t="n">
+      <c r="H16" s="1" t="n">
         <v>51991301817</v>
       </c>
       <c r="I16" s="0"/>
@@ -17083,28 +17041,28 @@
       <c r="AMJ16" s="0"/>
     </row>
     <row r="17" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
-      <c r="D17" s="6" t="s">
-        <v>33</v>
+      <c r="D17" s="1" t="s">
+        <v>34</v>
       </c>
-      <c r="E17" s="12" t="n">
+      <c r="E17" s="7" t="n">
         <v>5985368416</v>
       </c>
-      <c r="F17" s="13" t="s">
-        <v>34</v>
+      <c r="F17" s="8" t="s">
+        <v>35</v>
       </c>
-      <c r="G17" s="14" t="n">
+      <c r="G17" s="9" t="n">
         <v>31827</v>
       </c>
-      <c r="H17" s="8" t="n">
+      <c r="H17" s="1" t="n">
         <v>51991301817</v>
       </c>
       <c r="I17" s="0"/>
@@ -18125,28 +18083,28 @@
       <c r="AMJ17" s="0"/>
     </row>
     <row r="18" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="6" t="s">
+      <c r="A18" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
-      <c r="D18" s="6" t="s">
-        <v>35</v>
+      <c r="D18" s="1" t="s">
+        <v>36</v>
       </c>
-      <c r="E18" s="12" t="n">
+      <c r="E18" s="7" t="n">
         <v>70028986474</v>
       </c>
-      <c r="F18" s="13" t="s">
-        <v>36</v>
+      <c r="F18" s="8" t="s">
+        <v>37</v>
       </c>
-      <c r="G18" s="14" t="n">
+      <c r="G18" s="9" t="n">
         <v>34532</v>
       </c>
-      <c r="H18" s="8" t="n">
+      <c r="H18" s="1" t="n">
         <v>51991301817</v>
       </c>
       <c r="I18" s="0"/>
@@ -19167,28 +19125,28 @@
       <c r="AMJ18" s="0"/>
     </row>
     <row r="19" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="6" t="s">
+      <c r="A19" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
-      <c r="D19" s="6" t="s">
-        <v>37</v>
+      <c r="D19" s="1" t="s">
+        <v>38</v>
       </c>
-      <c r="E19" s="12" t="n">
+      <c r="E19" s="7" t="n">
         <v>6920673452</v>
       </c>
-      <c r="F19" s="13" t="s">
-        <v>38</v>
+      <c r="F19" s="8" t="s">
+        <v>39</v>
       </c>
-      <c r="G19" s="14" t="n">
+      <c r="G19" s="9" t="n">
         <v>31751</v>
       </c>
-      <c r="H19" s="8" t="n">
+      <c r="H19" s="1" t="n">
         <v>51991301817</v>
       </c>
       <c r="I19" s="0"/>
@@ -20209,28 +20167,28 @@
       <c r="AMJ19" s="0"/>
     </row>
     <row r="20" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="6" t="s">
+      <c r="A20" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
-      <c r="D20" s="6" t="s">
-        <v>39</v>
+      <c r="D20" s="1" t="s">
+        <v>40</v>
       </c>
-      <c r="E20" s="12" t="n">
+      <c r="E20" s="7" t="n">
         <v>2131</v>
       </c>
-      <c r="F20" s="13" t="s">
-        <v>40</v>
+      <c r="F20" s="8" t="s">
+        <v>41</v>
       </c>
-      <c r="G20" s="14" t="n">
+      <c r="G20" s="9" t="n">
         <v>30749</v>
       </c>
-      <c r="H20" s="8" t="n">
+      <c r="H20" s="1" t="n">
         <v>51991301817</v>
       </c>
       <c r="I20" s="0"/>
@@ -21250,14 +21208,1037 @@
       <c r="AMI20" s="0"/>
       <c r="AMJ20" s="0"/>
     </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="10"/>
+      <c r="B21" s="10"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="10"/>
+      <c r="I21" s="0"/>
+      <c r="J21" s="0"/>
+      <c r="K21" s="0"/>
+      <c r="L21" s="0"/>
+      <c r="M21" s="0"/>
+      <c r="N21" s="0"/>
+      <c r="O21" s="0"/>
+      <c r="P21" s="0"/>
+      <c r="Q21" s="0"/>
+      <c r="R21" s="0"/>
+      <c r="S21" s="0"/>
+      <c r="T21" s="0"/>
+      <c r="U21" s="0"/>
+      <c r="V21" s="0"/>
+      <c r="W21" s="0"/>
+      <c r="X21" s="0"/>
+      <c r="Y21" s="0"/>
+      <c r="Z21" s="0"/>
+      <c r="AA21" s="0"/>
+      <c r="AB21" s="0"/>
+      <c r="AC21" s="0"/>
+      <c r="AD21" s="0"/>
+      <c r="AE21" s="0"/>
+      <c r="AF21" s="0"/>
+      <c r="AG21" s="0"/>
+      <c r="AH21" s="0"/>
+      <c r="AI21" s="0"/>
+      <c r="AJ21" s="0"/>
+      <c r="AK21" s="0"/>
+      <c r="AL21" s="0"/>
+      <c r="AM21" s="0"/>
+      <c r="AN21" s="0"/>
+      <c r="AO21" s="0"/>
+      <c r="AP21" s="0"/>
+      <c r="AQ21" s="0"/>
+      <c r="AR21" s="0"/>
+      <c r="AS21" s="0"/>
+      <c r="AT21" s="0"/>
+      <c r="AU21" s="0"/>
+      <c r="AV21" s="0"/>
+      <c r="AW21" s="0"/>
+      <c r="AX21" s="0"/>
+      <c r="AY21" s="0"/>
+      <c r="AZ21" s="0"/>
+      <c r="BA21" s="0"/>
+      <c r="BB21" s="0"/>
+      <c r="BC21" s="0"/>
+      <c r="BD21" s="0"/>
+      <c r="BE21" s="0"/>
+      <c r="BF21" s="0"/>
+      <c r="BG21" s="0"/>
+      <c r="BH21" s="0"/>
+      <c r="BI21" s="0"/>
+      <c r="BJ21" s="0"/>
+      <c r="BK21" s="0"/>
+      <c r="BL21" s="0"/>
+      <c r="BM21" s="0"/>
+      <c r="BN21" s="0"/>
+      <c r="BO21" s="0"/>
+      <c r="BP21" s="0"/>
+      <c r="BQ21" s="0"/>
+      <c r="BR21" s="0"/>
+      <c r="BS21" s="0"/>
+      <c r="BT21" s="0"/>
+      <c r="BU21" s="0"/>
+      <c r="BV21" s="0"/>
+      <c r="BW21" s="0"/>
+      <c r="BX21" s="0"/>
+      <c r="BY21" s="0"/>
+      <c r="BZ21" s="0"/>
+      <c r="CA21" s="0"/>
+      <c r="CB21" s="0"/>
+      <c r="CC21" s="0"/>
+      <c r="CD21" s="0"/>
+      <c r="CE21" s="0"/>
+      <c r="CF21" s="0"/>
+      <c r="CG21" s="0"/>
+      <c r="CH21" s="0"/>
+      <c r="CI21" s="0"/>
+      <c r="CJ21" s="0"/>
+      <c r="CK21" s="0"/>
+      <c r="CL21" s="0"/>
+      <c r="CM21" s="0"/>
+      <c r="CN21" s="0"/>
+      <c r="CO21" s="0"/>
+      <c r="CP21" s="0"/>
+      <c r="CQ21" s="0"/>
+      <c r="CR21" s="0"/>
+      <c r="CS21" s="0"/>
+      <c r="CT21" s="0"/>
+      <c r="CU21" s="0"/>
+      <c r="CV21" s="0"/>
+      <c r="CW21" s="0"/>
+      <c r="CX21" s="0"/>
+      <c r="CY21" s="0"/>
+      <c r="CZ21" s="0"/>
+      <c r="DA21" s="0"/>
+      <c r="DB21" s="0"/>
+      <c r="DC21" s="0"/>
+      <c r="DD21" s="0"/>
+      <c r="DE21" s="0"/>
+      <c r="DF21" s="0"/>
+      <c r="DG21" s="0"/>
+      <c r="DH21" s="0"/>
+      <c r="DI21" s="0"/>
+      <c r="DJ21" s="0"/>
+      <c r="DK21" s="0"/>
+      <c r="DL21" s="0"/>
+      <c r="DM21" s="0"/>
+      <c r="DN21" s="0"/>
+      <c r="DO21" s="0"/>
+      <c r="DP21" s="0"/>
+      <c r="DQ21" s="0"/>
+      <c r="DR21" s="0"/>
+      <c r="DS21" s="0"/>
+      <c r="DT21" s="0"/>
+      <c r="DU21" s="0"/>
+      <c r="DV21" s="0"/>
+      <c r="DW21" s="0"/>
+      <c r="DX21" s="0"/>
+      <c r="DY21" s="0"/>
+      <c r="DZ21" s="0"/>
+      <c r="EA21" s="0"/>
+      <c r="EB21" s="0"/>
+      <c r="EC21" s="0"/>
+      <c r="ED21" s="0"/>
+      <c r="EE21" s="0"/>
+      <c r="EF21" s="0"/>
+      <c r="EG21" s="0"/>
+      <c r="EH21" s="0"/>
+      <c r="EI21" s="0"/>
+      <c r="EJ21" s="0"/>
+      <c r="EK21" s="0"/>
+      <c r="EL21" s="0"/>
+      <c r="EM21" s="0"/>
+      <c r="EN21" s="0"/>
+      <c r="EO21" s="0"/>
+      <c r="EP21" s="0"/>
+      <c r="EQ21" s="0"/>
+      <c r="ER21" s="0"/>
+      <c r="ES21" s="0"/>
+      <c r="ET21" s="0"/>
+      <c r="EU21" s="0"/>
+      <c r="EV21" s="0"/>
+      <c r="EW21" s="0"/>
+      <c r="EX21" s="0"/>
+      <c r="EY21" s="0"/>
+      <c r="EZ21" s="0"/>
+      <c r="FA21" s="0"/>
+      <c r="FB21" s="0"/>
+      <c r="FC21" s="0"/>
+      <c r="FD21" s="0"/>
+      <c r="FE21" s="0"/>
+      <c r="FF21" s="0"/>
+      <c r="FG21" s="0"/>
+      <c r="FH21" s="0"/>
+      <c r="FI21" s="0"/>
+      <c r="FJ21" s="0"/>
+      <c r="FK21" s="0"/>
+      <c r="FL21" s="0"/>
+      <c r="FM21" s="0"/>
+      <c r="FN21" s="0"/>
+      <c r="FO21" s="0"/>
+      <c r="FP21" s="0"/>
+      <c r="FQ21" s="0"/>
+      <c r="FR21" s="0"/>
+      <c r="FS21" s="0"/>
+      <c r="FT21" s="0"/>
+      <c r="FU21" s="0"/>
+      <c r="FV21" s="0"/>
+      <c r="FW21" s="0"/>
+      <c r="FX21" s="0"/>
+      <c r="FY21" s="0"/>
+      <c r="FZ21" s="0"/>
+      <c r="GA21" s="0"/>
+      <c r="GB21" s="0"/>
+      <c r="GC21" s="0"/>
+      <c r="GD21" s="0"/>
+      <c r="GE21" s="0"/>
+      <c r="GF21" s="0"/>
+      <c r="GG21" s="0"/>
+      <c r="GH21" s="0"/>
+      <c r="GI21" s="0"/>
+      <c r="GJ21" s="0"/>
+      <c r="GK21" s="0"/>
+      <c r="GL21" s="0"/>
+      <c r="GM21" s="0"/>
+      <c r="GN21" s="0"/>
+      <c r="GO21" s="0"/>
+      <c r="GP21" s="0"/>
+      <c r="GQ21" s="0"/>
+      <c r="GR21" s="0"/>
+      <c r="GS21" s="0"/>
+      <c r="GT21" s="0"/>
+      <c r="GU21" s="0"/>
+      <c r="GV21" s="0"/>
+      <c r="GW21" s="0"/>
+      <c r="GX21" s="0"/>
+      <c r="GY21" s="0"/>
+      <c r="GZ21" s="0"/>
+      <c r="HA21" s="0"/>
+      <c r="HB21" s="0"/>
+      <c r="HC21" s="0"/>
+      <c r="HD21" s="0"/>
+      <c r="HE21" s="0"/>
+      <c r="HF21" s="0"/>
+      <c r="HG21" s="0"/>
+      <c r="HH21" s="0"/>
+      <c r="HI21" s="0"/>
+      <c r="HJ21" s="0"/>
+      <c r="HK21" s="0"/>
+      <c r="HL21" s="0"/>
+      <c r="HM21" s="0"/>
+      <c r="HN21" s="0"/>
+      <c r="HO21" s="0"/>
+      <c r="HP21" s="0"/>
+      <c r="HQ21" s="0"/>
+      <c r="HR21" s="0"/>
+      <c r="HS21" s="0"/>
+      <c r="HT21" s="0"/>
+      <c r="HU21" s="0"/>
+      <c r="HV21" s="0"/>
+      <c r="HW21" s="0"/>
+      <c r="HX21" s="0"/>
+      <c r="HY21" s="0"/>
+      <c r="HZ21" s="0"/>
+      <c r="IA21" s="0"/>
+      <c r="IB21" s="0"/>
+      <c r="IC21" s="0"/>
+      <c r="ID21" s="0"/>
+      <c r="IE21" s="0"/>
+      <c r="IF21" s="0"/>
+      <c r="IG21" s="0"/>
+      <c r="IH21" s="0"/>
+      <c r="II21" s="0"/>
+      <c r="IJ21" s="0"/>
+      <c r="IK21" s="0"/>
+      <c r="IL21" s="0"/>
+      <c r="IM21" s="0"/>
+      <c r="IN21" s="0"/>
+      <c r="IO21" s="0"/>
+      <c r="IP21" s="0"/>
+      <c r="IQ21" s="0"/>
+      <c r="IR21" s="0"/>
+      <c r="IS21" s="0"/>
+      <c r="IT21" s="0"/>
+      <c r="IU21" s="0"/>
+      <c r="IV21" s="0"/>
+      <c r="IW21" s="0"/>
+      <c r="IX21" s="0"/>
+      <c r="IY21" s="0"/>
+      <c r="IZ21" s="0"/>
+      <c r="JA21" s="0"/>
+      <c r="JB21" s="0"/>
+      <c r="JC21" s="0"/>
+      <c r="JD21" s="0"/>
+      <c r="JE21" s="0"/>
+      <c r="JF21" s="0"/>
+      <c r="JG21" s="0"/>
+      <c r="JH21" s="0"/>
+      <c r="JI21" s="0"/>
+      <c r="JJ21" s="0"/>
+      <c r="JK21" s="0"/>
+      <c r="JL21" s="0"/>
+      <c r="JM21" s="0"/>
+      <c r="JN21" s="0"/>
+      <c r="JO21" s="0"/>
+      <c r="JP21" s="0"/>
+      <c r="JQ21" s="0"/>
+      <c r="JR21" s="0"/>
+      <c r="JS21" s="0"/>
+      <c r="JT21" s="0"/>
+      <c r="JU21" s="0"/>
+      <c r="JV21" s="0"/>
+      <c r="JW21" s="0"/>
+      <c r="JX21" s="0"/>
+      <c r="JY21" s="0"/>
+      <c r="JZ21" s="0"/>
+      <c r="KA21" s="0"/>
+      <c r="KB21" s="0"/>
+      <c r="KC21" s="0"/>
+      <c r="KD21" s="0"/>
+      <c r="KE21" s="0"/>
+      <c r="KF21" s="0"/>
+      <c r="KG21" s="0"/>
+      <c r="KH21" s="0"/>
+      <c r="KI21" s="0"/>
+      <c r="KJ21" s="0"/>
+      <c r="KK21" s="0"/>
+      <c r="KL21" s="0"/>
+      <c r="KM21" s="0"/>
+      <c r="KN21" s="0"/>
+      <c r="KO21" s="0"/>
+      <c r="KP21" s="0"/>
+      <c r="KQ21" s="0"/>
+      <c r="KR21" s="0"/>
+      <c r="KS21" s="0"/>
+      <c r="KT21" s="0"/>
+      <c r="KU21" s="0"/>
+      <c r="KV21" s="0"/>
+      <c r="KW21" s="0"/>
+      <c r="KX21" s="0"/>
+      <c r="KY21" s="0"/>
+      <c r="KZ21" s="0"/>
+      <c r="LA21" s="0"/>
+      <c r="LB21" s="0"/>
+      <c r="LC21" s="0"/>
+      <c r="LD21" s="0"/>
+      <c r="LE21" s="0"/>
+      <c r="LF21" s="0"/>
+      <c r="LG21" s="0"/>
+      <c r="LH21" s="0"/>
+      <c r="LI21" s="0"/>
+      <c r="LJ21" s="0"/>
+      <c r="LK21" s="0"/>
+      <c r="LL21" s="0"/>
+      <c r="LM21" s="0"/>
+      <c r="LN21" s="0"/>
+      <c r="LO21" s="0"/>
+      <c r="LP21" s="0"/>
+      <c r="LQ21" s="0"/>
+      <c r="LR21" s="0"/>
+      <c r="LS21" s="0"/>
+      <c r="LT21" s="0"/>
+      <c r="LU21" s="0"/>
+      <c r="LV21" s="0"/>
+      <c r="LW21" s="0"/>
+      <c r="LX21" s="0"/>
+      <c r="LY21" s="0"/>
+      <c r="LZ21" s="0"/>
+      <c r="MA21" s="0"/>
+      <c r="MB21" s="0"/>
+      <c r="MC21" s="0"/>
+      <c r="MD21" s="0"/>
+      <c r="ME21" s="0"/>
+      <c r="MF21" s="0"/>
+      <c r="MG21" s="0"/>
+      <c r="MH21" s="0"/>
+      <c r="MI21" s="0"/>
+      <c r="MJ21" s="0"/>
+      <c r="MK21" s="0"/>
+      <c r="ML21" s="0"/>
+      <c r="MM21" s="0"/>
+      <c r="MN21" s="0"/>
+      <c r="MO21" s="0"/>
+      <c r="MP21" s="0"/>
+      <c r="MQ21" s="0"/>
+      <c r="MR21" s="0"/>
+      <c r="MS21" s="0"/>
+      <c r="MT21" s="0"/>
+      <c r="MU21" s="0"/>
+      <c r="MV21" s="0"/>
+      <c r="MW21" s="0"/>
+      <c r="MX21" s="0"/>
+      <c r="MY21" s="0"/>
+      <c r="MZ21" s="0"/>
+      <c r="NA21" s="0"/>
+      <c r="NB21" s="0"/>
+      <c r="NC21" s="0"/>
+      <c r="ND21" s="0"/>
+      <c r="NE21" s="0"/>
+      <c r="NF21" s="0"/>
+      <c r="NG21" s="0"/>
+      <c r="NH21" s="0"/>
+      <c r="NI21" s="0"/>
+      <c r="NJ21" s="0"/>
+      <c r="NK21" s="0"/>
+      <c r="NL21" s="0"/>
+      <c r="NM21" s="0"/>
+      <c r="NN21" s="0"/>
+      <c r="NO21" s="0"/>
+      <c r="NP21" s="0"/>
+      <c r="NQ21" s="0"/>
+      <c r="NR21" s="0"/>
+      <c r="NS21" s="0"/>
+      <c r="NT21" s="0"/>
+      <c r="NU21" s="0"/>
+      <c r="NV21" s="0"/>
+      <c r="NW21" s="0"/>
+      <c r="NX21" s="0"/>
+      <c r="NY21" s="0"/>
+      <c r="NZ21" s="0"/>
+      <c r="OA21" s="0"/>
+      <c r="OB21" s="0"/>
+      <c r="OC21" s="0"/>
+      <c r="OD21" s="0"/>
+      <c r="OE21" s="0"/>
+      <c r="OF21" s="0"/>
+      <c r="OG21" s="0"/>
+      <c r="OH21" s="0"/>
+      <c r="OI21" s="0"/>
+      <c r="OJ21" s="0"/>
+      <c r="OK21" s="0"/>
+      <c r="OL21" s="0"/>
+      <c r="OM21" s="0"/>
+      <c r="ON21" s="0"/>
+      <c r="OO21" s="0"/>
+      <c r="OP21" s="0"/>
+      <c r="OQ21" s="0"/>
+      <c r="OR21" s="0"/>
+      <c r="OS21" s="0"/>
+      <c r="OT21" s="0"/>
+      <c r="OU21" s="0"/>
+      <c r="OV21" s="0"/>
+      <c r="OW21" s="0"/>
+      <c r="OX21" s="0"/>
+      <c r="OY21" s="0"/>
+      <c r="OZ21" s="0"/>
+      <c r="PA21" s="0"/>
+      <c r="PB21" s="0"/>
+      <c r="PC21" s="0"/>
+      <c r="PD21" s="0"/>
+      <c r="PE21" s="0"/>
+      <c r="PF21" s="0"/>
+      <c r="PG21" s="0"/>
+      <c r="PH21" s="0"/>
+      <c r="PI21" s="0"/>
+      <c r="PJ21" s="0"/>
+      <c r="PK21" s="0"/>
+      <c r="PL21" s="0"/>
+      <c r="PM21" s="0"/>
+      <c r="PN21" s="0"/>
+      <c r="PO21" s="0"/>
+      <c r="PP21" s="0"/>
+      <c r="PQ21" s="0"/>
+      <c r="PR21" s="0"/>
+      <c r="PS21" s="0"/>
+      <c r="PT21" s="0"/>
+      <c r="PU21" s="0"/>
+      <c r="PV21" s="0"/>
+      <c r="PW21" s="0"/>
+      <c r="PX21" s="0"/>
+      <c r="PY21" s="0"/>
+      <c r="PZ21" s="0"/>
+      <c r="QA21" s="0"/>
+      <c r="QB21" s="0"/>
+      <c r="QC21" s="0"/>
+      <c r="QD21" s="0"/>
+      <c r="QE21" s="0"/>
+      <c r="QF21" s="0"/>
+      <c r="QG21" s="0"/>
+      <c r="QH21" s="0"/>
+      <c r="QI21" s="0"/>
+      <c r="QJ21" s="0"/>
+      <c r="QK21" s="0"/>
+      <c r="QL21" s="0"/>
+      <c r="QM21" s="0"/>
+      <c r="QN21" s="0"/>
+      <c r="QO21" s="0"/>
+      <c r="QP21" s="0"/>
+      <c r="QQ21" s="0"/>
+      <c r="QR21" s="0"/>
+      <c r="QS21" s="0"/>
+      <c r="QT21" s="0"/>
+      <c r="QU21" s="0"/>
+      <c r="QV21" s="0"/>
+      <c r="QW21" s="0"/>
+      <c r="QX21" s="0"/>
+      <c r="QY21" s="0"/>
+      <c r="QZ21" s="0"/>
+      <c r="RA21" s="0"/>
+      <c r="RB21" s="0"/>
+      <c r="RC21" s="0"/>
+      <c r="RD21" s="0"/>
+      <c r="RE21" s="0"/>
+      <c r="RF21" s="0"/>
+      <c r="RG21" s="0"/>
+      <c r="RH21" s="0"/>
+      <c r="RI21" s="0"/>
+      <c r="RJ21" s="0"/>
+      <c r="RK21" s="0"/>
+      <c r="RL21" s="0"/>
+      <c r="RM21" s="0"/>
+      <c r="RN21" s="0"/>
+      <c r="RO21" s="0"/>
+      <c r="RP21" s="0"/>
+      <c r="RQ21" s="0"/>
+      <c r="RR21" s="0"/>
+      <c r="RS21" s="0"/>
+      <c r="RT21" s="0"/>
+      <c r="RU21" s="0"/>
+      <c r="RV21" s="0"/>
+      <c r="RW21" s="0"/>
+      <c r="RX21" s="0"/>
+      <c r="RY21" s="0"/>
+      <c r="RZ21" s="0"/>
+      <c r="SA21" s="0"/>
+      <c r="SB21" s="0"/>
+      <c r="SC21" s="0"/>
+      <c r="SD21" s="0"/>
+      <c r="SE21" s="0"/>
+      <c r="SF21" s="0"/>
+      <c r="SG21" s="0"/>
+      <c r="SH21" s="0"/>
+      <c r="SI21" s="0"/>
+      <c r="SJ21" s="0"/>
+      <c r="SK21" s="0"/>
+      <c r="SL21" s="0"/>
+      <c r="SM21" s="0"/>
+      <c r="SN21" s="0"/>
+      <c r="SO21" s="0"/>
+      <c r="SP21" s="0"/>
+      <c r="SQ21" s="0"/>
+      <c r="SR21" s="0"/>
+      <c r="SS21" s="0"/>
+      <c r="ST21" s="0"/>
+      <c r="SU21" s="0"/>
+      <c r="SV21" s="0"/>
+      <c r="SW21" s="0"/>
+      <c r="SX21" s="0"/>
+      <c r="SY21" s="0"/>
+      <c r="SZ21" s="0"/>
+      <c r="TA21" s="0"/>
+      <c r="TB21" s="0"/>
+      <c r="TC21" s="0"/>
+      <c r="TD21" s="0"/>
+      <c r="TE21" s="0"/>
+      <c r="TF21" s="0"/>
+      <c r="TG21" s="0"/>
+      <c r="TH21" s="0"/>
+      <c r="TI21" s="0"/>
+      <c r="TJ21" s="0"/>
+      <c r="TK21" s="0"/>
+      <c r="TL21" s="0"/>
+      <c r="TM21" s="0"/>
+      <c r="TN21" s="0"/>
+      <c r="TO21" s="0"/>
+      <c r="TP21" s="0"/>
+      <c r="TQ21" s="0"/>
+      <c r="TR21" s="0"/>
+      <c r="TS21" s="0"/>
+      <c r="TT21" s="0"/>
+      <c r="TU21" s="0"/>
+      <c r="TV21" s="0"/>
+      <c r="TW21" s="0"/>
+      <c r="TX21" s="0"/>
+      <c r="TY21" s="0"/>
+      <c r="TZ21" s="0"/>
+      <c r="UA21" s="0"/>
+      <c r="UB21" s="0"/>
+      <c r="UC21" s="0"/>
+      <c r="UD21" s="0"/>
+      <c r="UE21" s="0"/>
+      <c r="UF21" s="0"/>
+      <c r="UG21" s="0"/>
+      <c r="UH21" s="0"/>
+      <c r="UI21" s="0"/>
+      <c r="UJ21" s="0"/>
+      <c r="UK21" s="0"/>
+      <c r="UL21" s="0"/>
+      <c r="UM21" s="0"/>
+      <c r="UN21" s="0"/>
+      <c r="UO21" s="0"/>
+      <c r="UP21" s="0"/>
+      <c r="UQ21" s="0"/>
+      <c r="UR21" s="0"/>
+      <c r="US21" s="0"/>
+      <c r="UT21" s="0"/>
+      <c r="UU21" s="0"/>
+      <c r="UV21" s="0"/>
+      <c r="UW21" s="0"/>
+      <c r="UX21" s="0"/>
+      <c r="UY21" s="0"/>
+      <c r="UZ21" s="0"/>
+      <c r="VA21" s="0"/>
+      <c r="VB21" s="0"/>
+      <c r="VC21" s="0"/>
+      <c r="VD21" s="0"/>
+      <c r="VE21" s="0"/>
+      <c r="VF21" s="0"/>
+      <c r="VG21" s="0"/>
+      <c r="VH21" s="0"/>
+      <c r="VI21" s="0"/>
+      <c r="VJ21" s="0"/>
+      <c r="VK21" s="0"/>
+      <c r="VL21" s="0"/>
+      <c r="VM21" s="0"/>
+      <c r="VN21" s="0"/>
+      <c r="VO21" s="0"/>
+      <c r="VP21" s="0"/>
+      <c r="VQ21" s="0"/>
+      <c r="VR21" s="0"/>
+      <c r="VS21" s="0"/>
+      <c r="VT21" s="0"/>
+      <c r="VU21" s="0"/>
+      <c r="VV21" s="0"/>
+      <c r="VW21" s="0"/>
+      <c r="VX21" s="0"/>
+      <c r="VY21" s="0"/>
+      <c r="VZ21" s="0"/>
+      <c r="WA21" s="0"/>
+      <c r="WB21" s="0"/>
+      <c r="WC21" s="0"/>
+      <c r="WD21" s="0"/>
+      <c r="WE21" s="0"/>
+      <c r="WF21" s="0"/>
+      <c r="WG21" s="0"/>
+      <c r="WH21" s="0"/>
+      <c r="WI21" s="0"/>
+      <c r="WJ21" s="0"/>
+      <c r="WK21" s="0"/>
+      <c r="WL21" s="0"/>
+      <c r="WM21" s="0"/>
+      <c r="WN21" s="0"/>
+      <c r="WO21" s="0"/>
+      <c r="WP21" s="0"/>
+      <c r="WQ21" s="0"/>
+      <c r="WR21" s="0"/>
+      <c r="WS21" s="0"/>
+      <c r="WT21" s="0"/>
+      <c r="WU21" s="0"/>
+      <c r="WV21" s="0"/>
+      <c r="WW21" s="0"/>
+      <c r="WX21" s="0"/>
+      <c r="WY21" s="0"/>
+      <c r="WZ21" s="0"/>
+      <c r="XA21" s="0"/>
+      <c r="XB21" s="0"/>
+      <c r="XC21" s="0"/>
+      <c r="XD21" s="0"/>
+      <c r="XE21" s="0"/>
+      <c r="XF21" s="0"/>
+      <c r="XG21" s="0"/>
+      <c r="XH21" s="0"/>
+      <c r="XI21" s="0"/>
+      <c r="XJ21" s="0"/>
+      <c r="XK21" s="0"/>
+      <c r="XL21" s="0"/>
+      <c r="XM21" s="0"/>
+      <c r="XN21" s="0"/>
+      <c r="XO21" s="0"/>
+      <c r="XP21" s="0"/>
+      <c r="XQ21" s="0"/>
+      <c r="XR21" s="0"/>
+      <c r="XS21" s="0"/>
+      <c r="XT21" s="0"/>
+      <c r="XU21" s="0"/>
+      <c r="XV21" s="0"/>
+      <c r="XW21" s="0"/>
+      <c r="XX21" s="0"/>
+      <c r="XY21" s="0"/>
+      <c r="XZ21" s="0"/>
+      <c r="YA21" s="0"/>
+      <c r="YB21" s="0"/>
+      <c r="YC21" s="0"/>
+      <c r="YD21" s="0"/>
+      <c r="YE21" s="0"/>
+      <c r="YF21" s="0"/>
+      <c r="YG21" s="0"/>
+      <c r="YH21" s="0"/>
+      <c r="YI21" s="0"/>
+      <c r="YJ21" s="0"/>
+      <c r="YK21" s="0"/>
+      <c r="YL21" s="0"/>
+      <c r="YM21" s="0"/>
+      <c r="YN21" s="0"/>
+      <c r="YO21" s="0"/>
+      <c r="YP21" s="0"/>
+      <c r="YQ21" s="0"/>
+      <c r="YR21" s="0"/>
+      <c r="YS21" s="0"/>
+      <c r="YT21" s="0"/>
+      <c r="YU21" s="0"/>
+      <c r="YV21" s="0"/>
+      <c r="YW21" s="0"/>
+      <c r="YX21" s="0"/>
+      <c r="YY21" s="0"/>
+      <c r="YZ21" s="0"/>
+      <c r="ZA21" s="0"/>
+      <c r="ZB21" s="0"/>
+      <c r="ZC21" s="0"/>
+      <c r="ZD21" s="0"/>
+      <c r="ZE21" s="0"/>
+      <c r="ZF21" s="0"/>
+      <c r="ZG21" s="0"/>
+      <c r="ZH21" s="0"/>
+      <c r="ZI21" s="0"/>
+      <c r="ZJ21" s="0"/>
+      <c r="ZK21" s="0"/>
+      <c r="ZL21" s="0"/>
+      <c r="ZM21" s="0"/>
+      <c r="ZN21" s="0"/>
+      <c r="ZO21" s="0"/>
+      <c r="ZP21" s="0"/>
+      <c r="ZQ21" s="0"/>
+      <c r="ZR21" s="0"/>
+      <c r="ZS21" s="0"/>
+      <c r="ZT21" s="0"/>
+      <c r="ZU21" s="0"/>
+      <c r="ZV21" s="0"/>
+      <c r="ZW21" s="0"/>
+      <c r="ZX21" s="0"/>
+      <c r="ZY21" s="0"/>
+      <c r="ZZ21" s="0"/>
+      <c r="AAA21" s="0"/>
+      <c r="AAB21" s="0"/>
+      <c r="AAC21" s="0"/>
+      <c r="AAD21" s="0"/>
+      <c r="AAE21" s="0"/>
+      <c r="AAF21" s="0"/>
+      <c r="AAG21" s="0"/>
+      <c r="AAH21" s="0"/>
+      <c r="AAI21" s="0"/>
+      <c r="AAJ21" s="0"/>
+      <c r="AAK21" s="0"/>
+      <c r="AAL21" s="0"/>
+      <c r="AAM21" s="0"/>
+      <c r="AAN21" s="0"/>
+      <c r="AAO21" s="0"/>
+      <c r="AAP21" s="0"/>
+      <c r="AAQ21" s="0"/>
+      <c r="AAR21" s="0"/>
+      <c r="AAS21" s="0"/>
+      <c r="AAT21" s="0"/>
+      <c r="AAU21" s="0"/>
+      <c r="AAV21" s="0"/>
+      <c r="AAW21" s="0"/>
+      <c r="AAX21" s="0"/>
+      <c r="AAY21" s="0"/>
+      <c r="AAZ21" s="0"/>
+      <c r="ABA21" s="0"/>
+      <c r="ABB21" s="0"/>
+      <c r="ABC21" s="0"/>
+      <c r="ABD21" s="0"/>
+      <c r="ABE21" s="0"/>
+      <c r="ABF21" s="0"/>
+      <c r="ABG21" s="0"/>
+      <c r="ABH21" s="0"/>
+      <c r="ABI21" s="0"/>
+      <c r="ABJ21" s="0"/>
+      <c r="ABK21" s="0"/>
+      <c r="ABL21" s="0"/>
+      <c r="ABM21" s="0"/>
+      <c r="ABN21" s="0"/>
+      <c r="ABO21" s="0"/>
+      <c r="ABP21" s="0"/>
+      <c r="ABQ21" s="0"/>
+      <c r="ABR21" s="0"/>
+      <c r="ABS21" s="0"/>
+      <c r="ABT21" s="0"/>
+      <c r="ABU21" s="0"/>
+      <c r="ABV21" s="0"/>
+      <c r="ABW21" s="0"/>
+      <c r="ABX21" s="0"/>
+      <c r="ABY21" s="0"/>
+      <c r="ABZ21" s="0"/>
+      <c r="ACA21" s="0"/>
+      <c r="ACB21" s="0"/>
+      <c r="ACC21" s="0"/>
+      <c r="ACD21" s="0"/>
+      <c r="ACE21" s="0"/>
+      <c r="ACF21" s="0"/>
+      <c r="ACG21" s="0"/>
+      <c r="ACH21" s="0"/>
+      <c r="ACI21" s="0"/>
+      <c r="ACJ21" s="0"/>
+      <c r="ACK21" s="0"/>
+      <c r="ACL21" s="0"/>
+      <c r="ACM21" s="0"/>
+      <c r="ACN21" s="0"/>
+      <c r="ACO21" s="0"/>
+      <c r="ACP21" s="0"/>
+      <c r="ACQ21" s="0"/>
+      <c r="ACR21" s="0"/>
+      <c r="ACS21" s="0"/>
+      <c r="ACT21" s="0"/>
+      <c r="ACU21" s="0"/>
+      <c r="ACV21" s="0"/>
+      <c r="ACW21" s="0"/>
+      <c r="ACX21" s="0"/>
+      <c r="ACY21" s="0"/>
+      <c r="ACZ21" s="0"/>
+      <c r="ADA21" s="0"/>
+      <c r="ADB21" s="0"/>
+      <c r="ADC21" s="0"/>
+      <c r="ADD21" s="0"/>
+      <c r="ADE21" s="0"/>
+      <c r="ADF21" s="0"/>
+      <c r="ADG21" s="0"/>
+      <c r="ADH21" s="0"/>
+      <c r="ADI21" s="0"/>
+      <c r="ADJ21" s="0"/>
+      <c r="ADK21" s="0"/>
+      <c r="ADL21" s="0"/>
+      <c r="ADM21" s="0"/>
+      <c r="ADN21" s="0"/>
+      <c r="ADO21" s="0"/>
+      <c r="ADP21" s="0"/>
+      <c r="ADQ21" s="0"/>
+      <c r="ADR21" s="0"/>
+      <c r="ADS21" s="0"/>
+      <c r="ADT21" s="0"/>
+      <c r="ADU21" s="0"/>
+      <c r="ADV21" s="0"/>
+      <c r="ADW21" s="0"/>
+      <c r="ADX21" s="0"/>
+      <c r="ADY21" s="0"/>
+      <c r="ADZ21" s="0"/>
+      <c r="AEA21" s="0"/>
+      <c r="AEB21" s="0"/>
+      <c r="AEC21" s="0"/>
+      <c r="AED21" s="0"/>
+      <c r="AEE21" s="0"/>
+      <c r="AEF21" s="0"/>
+      <c r="AEG21" s="0"/>
+      <c r="AEH21" s="0"/>
+      <c r="AEI21" s="0"/>
+      <c r="AEJ21" s="0"/>
+      <c r="AEK21" s="0"/>
+      <c r="AEL21" s="0"/>
+      <c r="AEM21" s="0"/>
+      <c r="AEN21" s="0"/>
+      <c r="AEO21" s="0"/>
+      <c r="AEP21" s="0"/>
+      <c r="AEQ21" s="0"/>
+      <c r="AER21" s="0"/>
+      <c r="AES21" s="0"/>
+      <c r="AET21" s="0"/>
+      <c r="AEU21" s="0"/>
+      <c r="AEV21" s="0"/>
+      <c r="AEW21" s="0"/>
+      <c r="AEX21" s="0"/>
+      <c r="AEY21" s="0"/>
+      <c r="AEZ21" s="0"/>
+      <c r="AFA21" s="0"/>
+      <c r="AFB21" s="0"/>
+      <c r="AFC21" s="0"/>
+      <c r="AFD21" s="0"/>
+      <c r="AFE21" s="0"/>
+      <c r="AFF21" s="0"/>
+      <c r="AFG21" s="0"/>
+      <c r="AFH21" s="0"/>
+      <c r="AFI21" s="0"/>
+      <c r="AFJ21" s="0"/>
+      <c r="AFK21" s="0"/>
+      <c r="AFL21" s="0"/>
+      <c r="AFM21" s="0"/>
+      <c r="AFN21" s="0"/>
+      <c r="AFO21" s="0"/>
+      <c r="AFP21" s="0"/>
+      <c r="AFQ21" s="0"/>
+      <c r="AFR21" s="0"/>
+      <c r="AFS21" s="0"/>
+      <c r="AFT21" s="0"/>
+      <c r="AFU21" s="0"/>
+      <c r="AFV21" s="0"/>
+      <c r="AFW21" s="0"/>
+      <c r="AFX21" s="0"/>
+      <c r="AFY21" s="0"/>
+      <c r="AFZ21" s="0"/>
+      <c r="AGA21" s="0"/>
+      <c r="AGB21" s="0"/>
+      <c r="AGC21" s="0"/>
+      <c r="AGD21" s="0"/>
+      <c r="AGE21" s="0"/>
+      <c r="AGF21" s="0"/>
+      <c r="AGG21" s="0"/>
+      <c r="AGH21" s="0"/>
+      <c r="AGI21" s="0"/>
+      <c r="AGJ21" s="0"/>
+      <c r="AGK21" s="0"/>
+      <c r="AGL21" s="0"/>
+      <c r="AGM21" s="0"/>
+      <c r="AGN21" s="0"/>
+      <c r="AGO21" s="0"/>
+      <c r="AGP21" s="0"/>
+      <c r="AGQ21" s="0"/>
+      <c r="AGR21" s="0"/>
+      <c r="AGS21" s="0"/>
+      <c r="AGT21" s="0"/>
+      <c r="AGU21" s="0"/>
+      <c r="AGV21" s="0"/>
+      <c r="AGW21" s="0"/>
+      <c r="AGX21" s="0"/>
+      <c r="AGY21" s="0"/>
+      <c r="AGZ21" s="0"/>
+      <c r="AHA21" s="0"/>
+      <c r="AHB21" s="0"/>
+      <c r="AHC21" s="0"/>
+      <c r="AHD21" s="0"/>
+      <c r="AHE21" s="0"/>
+      <c r="AHF21" s="0"/>
+      <c r="AHG21" s="0"/>
+      <c r="AHH21" s="0"/>
+      <c r="AHI21" s="0"/>
+      <c r="AHJ21" s="0"/>
+      <c r="AHK21" s="0"/>
+      <c r="AHL21" s="0"/>
+      <c r="AHM21" s="0"/>
+      <c r="AHN21" s="0"/>
+      <c r="AHO21" s="0"/>
+      <c r="AHP21" s="0"/>
+      <c r="AHQ21" s="0"/>
+      <c r="AHR21" s="0"/>
+      <c r="AHS21" s="0"/>
+      <c r="AHT21" s="0"/>
+      <c r="AHU21" s="0"/>
+      <c r="AHV21" s="0"/>
+      <c r="AHW21" s="0"/>
+      <c r="AHX21" s="0"/>
+      <c r="AHY21" s="0"/>
+      <c r="AHZ21" s="0"/>
+      <c r="AIA21" s="0"/>
+      <c r="AIB21" s="0"/>
+      <c r="AIC21" s="0"/>
+      <c r="AID21" s="0"/>
+      <c r="AIE21" s="0"/>
+      <c r="AIF21" s="0"/>
+      <c r="AIG21" s="0"/>
+      <c r="AIH21" s="0"/>
+      <c r="AII21" s="0"/>
+      <c r="AIJ21" s="0"/>
+      <c r="AIK21" s="0"/>
+      <c r="AIL21" s="0"/>
+      <c r="AIM21" s="0"/>
+      <c r="AIN21" s="0"/>
+      <c r="AIO21" s="0"/>
+      <c r="AIP21" s="0"/>
+      <c r="AIQ21" s="0"/>
+      <c r="AIR21" s="0"/>
+      <c r="AIS21" s="0"/>
+      <c r="AIT21" s="0"/>
+      <c r="AIU21" s="0"/>
+      <c r="AIV21" s="0"/>
+      <c r="AIW21" s="0"/>
+      <c r="AIX21" s="0"/>
+      <c r="AIY21" s="0"/>
+      <c r="AIZ21" s="0"/>
+      <c r="AJA21" s="0"/>
+      <c r="AJB21" s="0"/>
+      <c r="AJC21" s="0"/>
+      <c r="AJD21" s="0"/>
+      <c r="AJE21" s="0"/>
+      <c r="AJF21" s="0"/>
+      <c r="AJG21" s="0"/>
+      <c r="AJH21" s="0"/>
+      <c r="AJI21" s="0"/>
+      <c r="AJJ21" s="0"/>
+      <c r="AJK21" s="0"/>
+      <c r="AJL21" s="0"/>
+      <c r="AJM21" s="0"/>
+      <c r="AJN21" s="0"/>
+      <c r="AJO21" s="0"/>
+      <c r="AJP21" s="0"/>
+      <c r="AJQ21" s="0"/>
+      <c r="AJR21" s="0"/>
+      <c r="AJS21" s="0"/>
+      <c r="AJT21" s="0"/>
+      <c r="AJU21" s="0"/>
+      <c r="AJV21" s="0"/>
+      <c r="AJW21" s="0"/>
+      <c r="AJX21" s="0"/>
+      <c r="AJY21" s="0"/>
+      <c r="AJZ21" s="0"/>
+      <c r="AKA21" s="0"/>
+      <c r="AKB21" s="0"/>
+      <c r="AKC21" s="0"/>
+      <c r="AKD21" s="0"/>
+      <c r="AKE21" s="0"/>
+      <c r="AKF21" s="0"/>
+      <c r="AKG21" s="0"/>
+      <c r="AKH21" s="0"/>
+      <c r="AKI21" s="0"/>
+      <c r="AKJ21" s="0"/>
+      <c r="AKK21" s="0"/>
+      <c r="AKL21" s="0"/>
+      <c r="AKM21" s="0"/>
+      <c r="AKN21" s="0"/>
+      <c r="AKO21" s="0"/>
+      <c r="AKP21" s="0"/>
+      <c r="AKQ21" s="0"/>
+      <c r="AKR21" s="0"/>
+      <c r="AKS21" s="0"/>
+      <c r="AKT21" s="0"/>
+      <c r="AKU21" s="0"/>
+      <c r="AKV21" s="0"/>
+      <c r="AKW21" s="0"/>
+      <c r="AKX21" s="0"/>
+      <c r="AKY21" s="0"/>
+      <c r="AKZ21" s="0"/>
+      <c r="ALA21" s="0"/>
+      <c r="ALB21" s="0"/>
+      <c r="ALC21" s="0"/>
+      <c r="ALD21" s="0"/>
+      <c r="ALE21" s="0"/>
+      <c r="ALF21" s="0"/>
+      <c r="ALG21" s="0"/>
+      <c r="ALH21" s="0"/>
+      <c r="ALI21" s="0"/>
+      <c r="ALJ21" s="0"/>
+      <c r="ALK21" s="0"/>
+      <c r="ALL21" s="0"/>
+      <c r="ALM21" s="0"/>
+      <c r="ALN21" s="0"/>
+      <c r="ALO21" s="0"/>
+      <c r="ALP21" s="0"/>
+      <c r="ALQ21" s="0"/>
+      <c r="ALR21" s="0"/>
+      <c r="ALS21" s="0"/>
+      <c r="ALT21" s="0"/>
+      <c r="ALU21" s="0"/>
+      <c r="ALV21" s="0"/>
+      <c r="ALW21" s="0"/>
+      <c r="ALX21" s="0"/>
+      <c r="ALY21" s="0"/>
+      <c r="ALZ21" s="0"/>
+      <c r="AMA21" s="0"/>
+      <c r="AMB21" s="0"/>
+      <c r="AMC21" s="0"/>
+      <c r="AMD21" s="0"/>
+      <c r="AME21" s="0"/>
+      <c r="AMF21" s="0"/>
+      <c r="AMG21" s="0"/>
+      <c r="AMH21" s="0"/>
+      <c r="AMI21" s="0"/>
+      <c r="AMJ21" s="0"/>
+    </row>
     <row r="22" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="6"/>
-      <c r="B22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="14"/>
-      <c r="H22" s="8"/>
+      <c r="C22" s="10"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="9"/>
       <c r="I22" s="0"/>
       <c r="J22" s="0"/>
       <c r="K22" s="0"/>
@@ -22276,13 +23257,10 @@
       <c r="AMJ22" s="0"/>
     </row>
     <row r="23" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="6"/>
-      <c r="B23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="14"/>
-      <c r="H23" s="8"/>
+      <c r="C23" s="10"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="9"/>
       <c r="I23" s="0"/>
       <c r="J23" s="0"/>
       <c r="K23" s="0"/>
@@ -23301,13 +24279,10 @@
       <c r="AMJ23" s="0"/>
     </row>
     <row r="24" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="6"/>
-      <c r="B24" s="6"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="12"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="14"/>
-      <c r="H24" s="8"/>
+      <c r="C24" s="10"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="8"/>
+      <c r="G24" s="9"/>
       <c r="I24" s="0"/>
       <c r="J24" s="0"/>
       <c r="K24" s="0"/>
@@ -24326,13 +25301,10 @@
       <c r="AMJ24" s="0"/>
     </row>
     <row r="25" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="6"/>
-      <c r="B25" s="6"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="12"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="14"/>
-      <c r="H25" s="8"/>
+      <c r="C25" s="10"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="8"/>
+      <c r="G25" s="9"/>
       <c r="I25" s="0"/>
       <c r="J25" s="0"/>
       <c r="K25" s="0"/>
@@ -25351,13 +26323,10 @@
       <c r="AMJ25" s="0"/>
     </row>
     <row r="26" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="6"/>
-      <c r="B26" s="6"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="12"/>
-      <c r="F26" s="13"/>
-      <c r="G26" s="14"/>
-      <c r="H26" s="8"/>
+      <c r="C26" s="10"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="8"/>
+      <c r="G26" s="9"/>
       <c r="I26" s="0"/>
       <c r="J26" s="0"/>
       <c r="K26" s="0"/>
@@ -26376,13 +27345,10 @@
       <c r="AMJ26" s="0"/>
     </row>
     <row r="27" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="6"/>
-      <c r="B27" s="6"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="12"/>
-      <c r="F27" s="13"/>
-      <c r="G27" s="14"/>
-      <c r="H27" s="8"/>
+      <c r="C27" s="10"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="8"/>
+      <c r="G27" s="9"/>
       <c r="I27" s="0"/>
       <c r="J27" s="0"/>
       <c r="K27" s="0"/>
@@ -27401,13 +28367,10 @@
       <c r="AMJ27" s="0"/>
     </row>
     <row r="28" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="6"/>
-      <c r="B28" s="6"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="12"/>
-      <c r="F28" s="13"/>
-      <c r="G28" s="14"/>
-      <c r="H28" s="8"/>
+      <c r="C28" s="10"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="8"/>
+      <c r="G28" s="9"/>
       <c r="I28" s="0"/>
       <c r="J28" s="0"/>
       <c r="K28" s="0"/>
@@ -28426,13 +29389,10 @@
       <c r="AMJ28" s="0"/>
     </row>
     <row r="29" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="6"/>
-      <c r="B29" s="6"/>
-      <c r="D29" s="6"/>
-      <c r="E29" s="12"/>
-      <c r="F29" s="13"/>
-      <c r="G29" s="14"/>
-      <c r="H29" s="8"/>
+      <c r="C29" s="10"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="8"/>
+      <c r="G29" s="9"/>
       <c r="I29" s="0"/>
       <c r="J29" s="0"/>
       <c r="K29" s="0"/>
@@ -29451,13 +30411,10 @@
       <c r="AMJ29" s="0"/>
     </row>
     <row r="30" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="6"/>
-      <c r="B30" s="6"/>
-      <c r="D30" s="6"/>
-      <c r="E30" s="12"/>
-      <c r="F30" s="13"/>
-      <c r="G30" s="14"/>
-      <c r="H30" s="8"/>
+      <c r="C30" s="10"/>
+      <c r="E30" s="7"/>
+      <c r="F30" s="8"/>
+      <c r="G30" s="9"/>
       <c r="I30" s="0"/>
       <c r="J30" s="0"/>
       <c r="K30" s="0"/>
@@ -30476,13 +31433,10 @@
       <c r="AMJ30" s="0"/>
     </row>
     <row r="31" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="6"/>
-      <c r="B31" s="6"/>
-      <c r="D31" s="6"/>
-      <c r="E31" s="12"/>
-      <c r="F31" s="13"/>
-      <c r="G31" s="14"/>
-      <c r="H31" s="8"/>
+      <c r="C31" s="10"/>
+      <c r="E31" s="7"/>
+      <c r="F31" s="8"/>
+      <c r="G31" s="9"/>
       <c r="I31" s="0"/>
       <c r="J31" s="0"/>
       <c r="K31" s="0"/>
@@ -31501,13 +32455,10 @@
       <c r="AMJ31" s="0"/>
     </row>
     <row r="32" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="6"/>
-      <c r="B32" s="6"/>
-      <c r="D32" s="6"/>
-      <c r="E32" s="12"/>
-      <c r="F32" s="13"/>
-      <c r="G32" s="14"/>
-      <c r="H32" s="8"/>
+      <c r="C32" s="10"/>
+      <c r="E32" s="7"/>
+      <c r="F32" s="8"/>
+      <c r="G32" s="9"/>
       <c r="I32" s="0"/>
       <c r="J32" s="0"/>
       <c r="K32" s="0"/>
@@ -32526,13 +33477,10 @@
       <c r="AMJ32" s="0"/>
     </row>
     <row r="33" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="6"/>
-      <c r="B33" s="6"/>
-      <c r="D33" s="6"/>
-      <c r="E33" s="12"/>
-      <c r="F33" s="13"/>
-      <c r="G33" s="14"/>
-      <c r="H33" s="8"/>
+      <c r="C33" s="10"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="8"/>
+      <c r="G33" s="9"/>
       <c r="I33" s="0"/>
       <c r="J33" s="0"/>
       <c r="K33" s="0"/>
@@ -33551,13 +34499,10 @@
       <c r="AMJ33" s="0"/>
     </row>
     <row r="34" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="6"/>
-      <c r="B34" s="6"/>
-      <c r="D34" s="6"/>
-      <c r="E34" s="12"/>
-      <c r="F34" s="13"/>
-      <c r="G34" s="14"/>
-      <c r="H34" s="8"/>
+      <c r="C34" s="10"/>
+      <c r="E34" s="7"/>
+      <c r="F34" s="8"/>
+      <c r="G34" s="9"/>
       <c r="I34" s="0"/>
       <c r="J34" s="0"/>
       <c r="K34" s="0"/>
@@ -34576,13 +35521,10 @@
       <c r="AMJ34" s="0"/>
     </row>
     <row r="35" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="6"/>
-      <c r="B35" s="6"/>
-      <c r="D35" s="6"/>
-      <c r="E35" s="12"/>
-      <c r="F35" s="13"/>
-      <c r="G35" s="14"/>
-      <c r="H35" s="8"/>
+      <c r="C35" s="10"/>
+      <c r="E35" s="7"/>
+      <c r="F35" s="8"/>
+      <c r="G35" s="9"/>
       <c r="I35" s="0"/>
       <c r="J35" s="0"/>
       <c r="K35" s="0"/>
@@ -35601,13 +36543,10 @@
       <c r="AMJ35" s="0"/>
     </row>
     <row r="36" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="6"/>
-      <c r="B36" s="6"/>
-      <c r="D36" s="6"/>
-      <c r="E36" s="12"/>
-      <c r="F36" s="13"/>
-      <c r="G36" s="14"/>
-      <c r="H36" s="8"/>
+      <c r="C36" s="10"/>
+      <c r="E36" s="7"/>
+      <c r="F36" s="8"/>
+      <c r="G36" s="9"/>
       <c r="I36" s="0"/>
       <c r="J36" s="0"/>
       <c r="K36" s="0"/>
@@ -36626,13 +37565,10 @@
       <c r="AMJ36" s="0"/>
     </row>
     <row r="37" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="6"/>
-      <c r="B37" s="6"/>
-      <c r="D37" s="6"/>
-      <c r="E37" s="12"/>
-      <c r="F37" s="13"/>
-      <c r="G37" s="14"/>
-      <c r="H37" s="8"/>
+      <c r="C37" s="10"/>
+      <c r="E37" s="7"/>
+      <c r="F37" s="8"/>
+      <c r="G37" s="9"/>
       <c r="I37" s="0"/>
       <c r="J37" s="0"/>
       <c r="K37" s="0"/>
@@ -37651,13 +38587,10 @@
       <c r="AMJ37" s="0"/>
     </row>
     <row r="38" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="6"/>
-      <c r="B38" s="6"/>
-      <c r="D38" s="6"/>
-      <c r="E38" s="12"/>
-      <c r="F38" s="13"/>
-      <c r="G38" s="14"/>
-      <c r="H38" s="8"/>
+      <c r="C38" s="10"/>
+      <c r="E38" s="7"/>
+      <c r="F38" s="8"/>
+      <c r="G38" s="9"/>
       <c r="I38" s="0"/>
       <c r="J38" s="0"/>
       <c r="K38" s="0"/>
@@ -38676,13 +39609,10 @@
       <c r="AMJ38" s="0"/>
     </row>
     <row r="39" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="6"/>
-      <c r="B39" s="6"/>
-      <c r="D39" s="6"/>
-      <c r="E39" s="12"/>
-      <c r="F39" s="13"/>
-      <c r="G39" s="14"/>
-      <c r="H39" s="8"/>
+      <c r="C39" s="10"/>
+      <c r="E39" s="7"/>
+      <c r="F39" s="8"/>
+      <c r="G39" s="9"/>
       <c r="I39" s="0"/>
       <c r="J39" s="0"/>
       <c r="K39" s="0"/>
@@ -39701,13 +40631,10 @@
       <c r="AMJ39" s="0"/>
     </row>
     <row r="40" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A40" s="6"/>
-      <c r="B40" s="6"/>
-      <c r="D40" s="6"/>
-      <c r="E40" s="12"/>
-      <c r="F40" s="13"/>
-      <c r="G40" s="14"/>
-      <c r="H40" s="8"/>
+      <c r="C40" s="10"/>
+      <c r="E40" s="7"/>
+      <c r="F40" s="8"/>
+      <c r="G40" s="9"/>
       <c r="I40" s="0"/>
       <c r="J40" s="0"/>
       <c r="K40" s="0"/>
@@ -40726,13 +41653,10 @@
       <c r="AMJ40" s="0"/>
     </row>
     <row r="41" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A41" s="6"/>
-      <c r="B41" s="6"/>
-      <c r="D41" s="6"/>
-      <c r="E41" s="12"/>
-      <c r="F41" s="13"/>
-      <c r="G41" s="14"/>
-      <c r="H41" s="8"/>
+      <c r="C41" s="10"/>
+      <c r="E41" s="7"/>
+      <c r="F41" s="8"/>
+      <c r="G41" s="9"/>
       <c r="I41" s="0"/>
       <c r="J41" s="0"/>
       <c r="K41" s="0"/>
@@ -41751,13 +42675,10 @@
       <c r="AMJ41" s="0"/>
     </row>
     <row r="42" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A42" s="6"/>
-      <c r="B42" s="6"/>
-      <c r="D42" s="6"/>
-      <c r="E42" s="12"/>
-      <c r="F42" s="13"/>
-      <c r="G42" s="14"/>
-      <c r="H42" s="8"/>
+      <c r="C42" s="10"/>
+      <c r="E42" s="7"/>
+      <c r="F42" s="8"/>
+      <c r="G42" s="9"/>
       <c r="I42" s="0"/>
       <c r="J42" s="0"/>
       <c r="K42" s="0"/>
@@ -42776,13 +43697,10 @@
       <c r="AMJ42" s="0"/>
     </row>
     <row r="43" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A43" s="6"/>
-      <c r="B43" s="6"/>
-      <c r="D43" s="6"/>
-      <c r="E43" s="12"/>
-      <c r="F43" s="13"/>
-      <c r="G43" s="14"/>
-      <c r="H43" s="8"/>
+      <c r="C43" s="10"/>
+      <c r="E43" s="7"/>
+      <c r="F43" s="8"/>
+      <c r="G43" s="9"/>
       <c r="I43" s="0"/>
       <c r="J43" s="0"/>
       <c r="K43" s="0"/>
@@ -43801,13 +44719,10 @@
       <c r="AMJ43" s="0"/>
     </row>
     <row r="44" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A44" s="6"/>
-      <c r="B44" s="6"/>
-      <c r="D44" s="6"/>
-      <c r="E44" s="12"/>
-      <c r="F44" s="13"/>
-      <c r="G44" s="14"/>
-      <c r="H44" s="8"/>
+      <c r="C44" s="10"/>
+      <c r="E44" s="7"/>
+      <c r="F44" s="8"/>
+      <c r="G44" s="9"/>
       <c r="I44" s="0"/>
       <c r="J44" s="0"/>
       <c r="K44" s="0"/>
@@ -44826,13 +45741,10 @@
       <c r="AMJ44" s="0"/>
     </row>
     <row r="45" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A45" s="6"/>
-      <c r="B45" s="6"/>
-      <c r="D45" s="6"/>
-      <c r="E45" s="12"/>
-      <c r="F45" s="13"/>
-      <c r="G45" s="14"/>
-      <c r="H45" s="8"/>
+      <c r="C45" s="10"/>
+      <c r="E45" s="7"/>
+      <c r="F45" s="8"/>
+      <c r="G45" s="9"/>
       <c r="I45" s="0"/>
       <c r="J45" s="0"/>
       <c r="K45" s="0"/>
@@ -45851,13 +46763,10 @@
       <c r="AMJ45" s="0"/>
     </row>
     <row r="46" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A46" s="6"/>
-      <c r="B46" s="6"/>
-      <c r="D46" s="6"/>
-      <c r="E46" s="12"/>
-      <c r="F46" s="13"/>
-      <c r="G46" s="14"/>
-      <c r="H46" s="8"/>
+      <c r="C46" s="10"/>
+      <c r="E46" s="7"/>
+      <c r="F46" s="8"/>
+      <c r="G46" s="9"/>
       <c r="I46" s="0"/>
       <c r="J46" s="0"/>
       <c r="K46" s="0"/>
@@ -46876,13 +47785,10 @@
       <c r="AMJ46" s="0"/>
     </row>
     <row r="47" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A47" s="6"/>
-      <c r="B47" s="6"/>
-      <c r="D47" s="6"/>
-      <c r="E47" s="12"/>
-      <c r="F47" s="13"/>
-      <c r="G47" s="14"/>
-      <c r="H47" s="8"/>
+      <c r="C47" s="10"/>
+      <c r="E47" s="7"/>
+      <c r="F47" s="8"/>
+      <c r="G47" s="9"/>
       <c r="I47" s="0"/>
       <c r="J47" s="0"/>
       <c r="K47" s="0"/>
@@ -47901,13 +48807,10 @@
       <c r="AMJ47" s="0"/>
     </row>
     <row r="48" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A48" s="6"/>
-      <c r="B48" s="6"/>
-      <c r="D48" s="6"/>
-      <c r="E48" s="12"/>
-      <c r="F48" s="13"/>
-      <c r="G48" s="14"/>
-      <c r="H48" s="8"/>
+      <c r="C48" s="10"/>
+      <c r="E48" s="7"/>
+      <c r="F48" s="8"/>
+      <c r="G48" s="9"/>
       <c r="I48" s="0"/>
       <c r="J48" s="0"/>
       <c r="K48" s="0"/>
@@ -48926,28 +49829,28 @@
       <c r="AMJ48" s="0"/>
     </row>
     <row r="49" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A49" s="6" t="s">
+      <c r="A49" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B49" s="6" t="s">
+      <c r="B49" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
-      <c r="D49" s="6" t="s">
-        <v>41</v>
+      <c r="D49" s="1" t="s">
+        <v>42</v>
       </c>
-      <c r="E49" s="12" t="n">
+      <c r="E49" s="7" t="n">
         <v>9460873421</v>
       </c>
-      <c r="F49" s="13" t="s">
-        <v>42</v>
+      <c r="F49" s="8" t="s">
+        <v>43</v>
       </c>
-      <c r="G49" s="14" t="n">
+      <c r="G49" s="9" t="n">
         <v>34055</v>
       </c>
-      <c r="H49" s="8" t="n">
+      <c r="H49" s="1" t="n">
         <v>51991301817</v>
       </c>
       <c r="I49" s="0"/>
@@ -50095,16 +50998,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="8.10204081632653"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="31.3163265306122"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.10204081632653"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.9132653061224"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.1224489795918"/>
   </cols>
   <sheetData>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D4" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F4" s="0" t="s">
         <v>9</v>
@@ -50112,35 +51012,35 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D5" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D6" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D7" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D8" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D9" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D10" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -50150,12 +51050,12 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D12" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D13" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
#10445 - Modifica arquivo para testes
</commit_message>
<xml_diff>
--- a/src/test/resources/arquivo_usuario/planilha.xlsx
+++ b/src/test/resources/arquivo_usuario/planilha.xlsx
@@ -451,12 +451,12 @@
   <dimension ref="1:49"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I7" activeCellId="0" sqref="I7"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="4:4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="19.4489795918367"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="12.4183673469388"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="1" width="18.4948979591837"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="1" width="45.3571428571429"/>
@@ -50993,7 +50993,7 @@
   <dimension ref="D4:F13"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
+      <selection pane="topLeft" activeCell="E15" activeCellId="1" sqref="4:4 E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Trata quando ocorre erro ao receber uma data invalida
</commit_message>
<xml_diff>
--- a/src/test/resources/arquivo_usuario/planilha.xlsx
+++ b/src/test/resources/arquivo_usuario/planilha.xlsx
@@ -450,24 +450,17 @@
   </sheetPr>
   <dimension ref="1:49"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="4:4"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="A:H"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="19.4489795918367"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="18.4948979591837"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="45.3571428571429"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="30.6428571428571"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="20.25"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="14" min="9" style="2" width="7.1530612244898"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="2" width="18.765306122449"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="2" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="1025" min="17" style="2" width="7.1530612244898"/>
+    <col collapsed="false" hidden="false" max="8" min="1" style="1" width="36.1224489795918"/>
+    <col collapsed="false" hidden="false" max="14" min="9" style="2" width="6.88265306122449"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="2" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="2" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="1025" min="17" style="2" width="6.88265306122449"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3594,7 +3587,7 @@
       <c r="AMI3" s="0"/>
       <c r="AMJ3" s="0"/>
     </row>
-    <row r="4" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
@@ -4636,7 +4629,7 @@
       <c r="AMI4" s="0"/>
       <c r="AMJ4" s="0"/>
     </row>
-    <row r="5" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -5678,7 +5671,7 @@
       <c r="AMI5" s="0"/>
       <c r="AMJ5" s="0"/>
     </row>
-    <row r="6" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -6720,7 +6713,7 @@
       <c r="AMI6" s="0"/>
       <c r="AMJ6" s="0"/>
     </row>
-    <row r="7" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -7762,7 +7755,7 @@
       <c r="AMI7" s="0"/>
       <c r="AMJ7" s="0"/>
     </row>
-    <row r="8" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
@@ -8804,7 +8797,7 @@
       <c r="AMI8" s="0"/>
       <c r="AMJ8" s="0"/>
     </row>
-    <row r="9" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -9846,7 +9839,7 @@
       <c r="AMI9" s="0"/>
       <c r="AMJ9" s="0"/>
     </row>
-    <row r="10" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -10888,11 +10881,15 @@
       <c r="AMI10" s="0"/>
       <c r="AMJ10" s="0"/>
     </row>
-    <row r="11" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="10"/>
+      <c r="B11" s="10"/>
       <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
       <c r="E11" s="7"/>
       <c r="F11" s="8"/>
       <c r="G11" s="9"/>
+      <c r="H11" s="10"/>
       <c r="I11" s="0"/>
       <c r="J11" s="0"/>
       <c r="K11" s="0"/>
@@ -11910,11 +11907,15 @@
       <c r="AMI11" s="0"/>
       <c r="AMJ11" s="0"/>
     </row>
-    <row r="12" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="10"/>
+      <c r="B12" s="10"/>
       <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
       <c r="E12" s="7"/>
       <c r="F12" s="8"/>
       <c r="G12" s="9"/>
+      <c r="H12" s="10"/>
       <c r="I12" s="0"/>
       <c r="J12" s="0"/>
       <c r="K12" s="0"/>
@@ -12932,11 +12933,15 @@
       <c r="AMI12" s="0"/>
       <c r="AMJ12" s="0"/>
     </row>
-    <row r="13" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="10"/>
+      <c r="B13" s="10"/>
       <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
       <c r="E13" s="7"/>
       <c r="F13" s="8"/>
       <c r="G13" s="9"/>
+      <c r="H13" s="10"/>
       <c r="I13" s="0"/>
       <c r="J13" s="0"/>
       <c r="K13" s="0"/>
@@ -13954,11 +13959,15 @@
       <c r="AMI13" s="0"/>
       <c r="AMJ13" s="0"/>
     </row>
-    <row r="14" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="10"/>
+      <c r="B14" s="10"/>
       <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
       <c r="E14" s="7"/>
       <c r="F14" s="8"/>
       <c r="G14" s="9"/>
+      <c r="H14" s="10"/>
       <c r="I14" s="0"/>
       <c r="J14" s="0"/>
       <c r="K14" s="0"/>
@@ -14976,11 +14985,15 @@
       <c r="AMI14" s="0"/>
       <c r="AMJ14" s="0"/>
     </row>
-    <row r="15" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="10"/>
+      <c r="B15" s="10"/>
       <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
       <c r="E15" s="7"/>
       <c r="F15" s="8"/>
       <c r="G15" s="9"/>
+      <c r="H15" s="10"/>
       <c r="I15" s="0"/>
       <c r="J15" s="0"/>
       <c r="K15" s="0"/>
@@ -15998,7 +16011,7 @@
       <c r="AMI15" s="0"/>
       <c r="AMJ15" s="0"/>
     </row>
-    <row r="16" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
         <v>8</v>
       </c>
@@ -17040,7 +17053,7 @@
       <c r="AMI16" s="0"/>
       <c r="AMJ16" s="0"/>
     </row>
-    <row r="17" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
         <v>8</v>
       </c>
@@ -18082,7 +18095,7 @@
       <c r="AMI17" s="0"/>
       <c r="AMJ17" s="0"/>
     </row>
-    <row r="18" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
         <v>8</v>
       </c>
@@ -19124,7 +19137,7 @@
       <c r="AMI18" s="0"/>
       <c r="AMJ18" s="0"/>
     </row>
-    <row r="19" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
         <v>8</v>
       </c>
@@ -20166,7 +20179,7 @@
       <c r="AMI19" s="0"/>
       <c r="AMJ19" s="0"/>
     </row>
-    <row r="20" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
         <v>8</v>
       </c>
@@ -22234,11 +22247,15 @@
       <c r="AMI21" s="0"/>
       <c r="AMJ21" s="0"/>
     </row>
-    <row r="22" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="10"/>
+      <c r="B22" s="10"/>
       <c r="C22" s="10"/>
+      <c r="D22" s="10"/>
       <c r="E22" s="7"/>
       <c r="F22" s="8"/>
       <c r="G22" s="9"/>
+      <c r="H22" s="10"/>
       <c r="I22" s="0"/>
       <c r="J22" s="0"/>
       <c r="K22" s="0"/>
@@ -23256,11 +23273,15 @@
       <c r="AMI22" s="0"/>
       <c r="AMJ22" s="0"/>
     </row>
-    <row r="23" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="10"/>
+      <c r="B23" s="10"/>
       <c r="C23" s="10"/>
+      <c r="D23" s="10"/>
       <c r="E23" s="7"/>
       <c r="F23" s="8"/>
       <c r="G23" s="9"/>
+      <c r="H23" s="10"/>
       <c r="I23" s="0"/>
       <c r="J23" s="0"/>
       <c r="K23" s="0"/>
@@ -24278,11 +24299,15 @@
       <c r="AMI23" s="0"/>
       <c r="AMJ23" s="0"/>
     </row>
-    <row r="24" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="10"/>
+      <c r="B24" s="10"/>
       <c r="C24" s="10"/>
+      <c r="D24" s="10"/>
       <c r="E24" s="7"/>
       <c r="F24" s="8"/>
       <c r="G24" s="9"/>
+      <c r="H24" s="10"/>
       <c r="I24" s="0"/>
       <c r="J24" s="0"/>
       <c r="K24" s="0"/>
@@ -25300,11 +25325,15 @@
       <c r="AMI24" s="0"/>
       <c r="AMJ24" s="0"/>
     </row>
-    <row r="25" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="10"/>
+      <c r="B25" s="10"/>
       <c r="C25" s="10"/>
+      <c r="D25" s="10"/>
       <c r="E25" s="7"/>
       <c r="F25" s="8"/>
       <c r="G25" s="9"/>
+      <c r="H25" s="10"/>
       <c r="I25" s="0"/>
       <c r="J25" s="0"/>
       <c r="K25" s="0"/>
@@ -26322,11 +26351,15 @@
       <c r="AMI25" s="0"/>
       <c r="AMJ25" s="0"/>
     </row>
-    <row r="26" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="10"/>
+      <c r="B26" s="10"/>
       <c r="C26" s="10"/>
+      <c r="D26" s="10"/>
       <c r="E26" s="7"/>
       <c r="F26" s="8"/>
       <c r="G26" s="9"/>
+      <c r="H26" s="10"/>
       <c r="I26" s="0"/>
       <c r="J26" s="0"/>
       <c r="K26" s="0"/>
@@ -27344,11 +27377,15 @@
       <c r="AMI26" s="0"/>
       <c r="AMJ26" s="0"/>
     </row>
-    <row r="27" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="10"/>
+      <c r="B27" s="10"/>
       <c r="C27" s="10"/>
+      <c r="D27" s="10"/>
       <c r="E27" s="7"/>
       <c r="F27" s="8"/>
       <c r="G27" s="9"/>
+      <c r="H27" s="10"/>
       <c r="I27" s="0"/>
       <c r="J27" s="0"/>
       <c r="K27" s="0"/>
@@ -28366,11 +28403,15 @@
       <c r="AMI27" s="0"/>
       <c r="AMJ27" s="0"/>
     </row>
-    <row r="28" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="10"/>
+      <c r="B28" s="10"/>
       <c r="C28" s="10"/>
+      <c r="D28" s="10"/>
       <c r="E28" s="7"/>
       <c r="F28" s="8"/>
       <c r="G28" s="9"/>
+      <c r="H28" s="10"/>
       <c r="I28" s="0"/>
       <c r="J28" s="0"/>
       <c r="K28" s="0"/>
@@ -29388,11 +29429,15 @@
       <c r="AMI28" s="0"/>
       <c r="AMJ28" s="0"/>
     </row>
-    <row r="29" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="10"/>
+      <c r="B29" s="10"/>
       <c r="C29" s="10"/>
+      <c r="D29" s="10"/>
       <c r="E29" s="7"/>
       <c r="F29" s="8"/>
       <c r="G29" s="9"/>
+      <c r="H29" s="10"/>
       <c r="I29" s="0"/>
       <c r="J29" s="0"/>
       <c r="K29" s="0"/>
@@ -30410,11 +30455,15 @@
       <c r="AMI29" s="0"/>
       <c r="AMJ29" s="0"/>
     </row>
-    <row r="30" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="10"/>
+      <c r="B30" s="10"/>
       <c r="C30" s="10"/>
+      <c r="D30" s="10"/>
       <c r="E30" s="7"/>
       <c r="F30" s="8"/>
       <c r="G30" s="9"/>
+      <c r="H30" s="10"/>
       <c r="I30" s="0"/>
       <c r="J30" s="0"/>
       <c r="K30" s="0"/>
@@ -31432,11 +31481,15 @@
       <c r="AMI30" s="0"/>
       <c r="AMJ30" s="0"/>
     </row>
-    <row r="31" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="10"/>
+      <c r="B31" s="10"/>
       <c r="C31" s="10"/>
+      <c r="D31" s="10"/>
       <c r="E31" s="7"/>
       <c r="F31" s="8"/>
       <c r="G31" s="9"/>
+      <c r="H31" s="10"/>
       <c r="I31" s="0"/>
       <c r="J31" s="0"/>
       <c r="K31" s="0"/>
@@ -32454,11 +32507,15 @@
       <c r="AMI31" s="0"/>
       <c r="AMJ31" s="0"/>
     </row>
-    <row r="32" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="10"/>
+      <c r="B32" s="10"/>
       <c r="C32" s="10"/>
+      <c r="D32" s="10"/>
       <c r="E32" s="7"/>
       <c r="F32" s="8"/>
       <c r="G32" s="9"/>
+      <c r="H32" s="10"/>
       <c r="I32" s="0"/>
       <c r="J32" s="0"/>
       <c r="K32" s="0"/>
@@ -33476,11 +33533,15 @@
       <c r="AMI32" s="0"/>
       <c r="AMJ32" s="0"/>
     </row>
-    <row r="33" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="10"/>
+      <c r="B33" s="10"/>
       <c r="C33" s="10"/>
+      <c r="D33" s="10"/>
       <c r="E33" s="7"/>
       <c r="F33" s="8"/>
       <c r="G33" s="9"/>
+      <c r="H33" s="10"/>
       <c r="I33" s="0"/>
       <c r="J33" s="0"/>
       <c r="K33" s="0"/>
@@ -34498,11 +34559,15 @@
       <c r="AMI33" s="0"/>
       <c r="AMJ33" s="0"/>
     </row>
-    <row r="34" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="10"/>
+      <c r="B34" s="10"/>
       <c r="C34" s="10"/>
+      <c r="D34" s="10"/>
       <c r="E34" s="7"/>
       <c r="F34" s="8"/>
       <c r="G34" s="9"/>
+      <c r="H34" s="10"/>
       <c r="I34" s="0"/>
       <c r="J34" s="0"/>
       <c r="K34" s="0"/>
@@ -35520,11 +35585,15 @@
       <c r="AMI34" s="0"/>
       <c r="AMJ34" s="0"/>
     </row>
-    <row r="35" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="10"/>
+      <c r="B35" s="10"/>
       <c r="C35" s="10"/>
+      <c r="D35" s="10"/>
       <c r="E35" s="7"/>
       <c r="F35" s="8"/>
       <c r="G35" s="9"/>
+      <c r="H35" s="10"/>
       <c r="I35" s="0"/>
       <c r="J35" s="0"/>
       <c r="K35" s="0"/>
@@ -36542,11 +36611,15 @@
       <c r="AMI35" s="0"/>
       <c r="AMJ35" s="0"/>
     </row>
-    <row r="36" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="10"/>
+      <c r="B36" s="10"/>
       <c r="C36" s="10"/>
+      <c r="D36" s="10"/>
       <c r="E36" s="7"/>
       <c r="F36" s="8"/>
       <c r="G36" s="9"/>
+      <c r="H36" s="10"/>
       <c r="I36" s="0"/>
       <c r="J36" s="0"/>
       <c r="K36" s="0"/>
@@ -37564,11 +37637,15 @@
       <c r="AMI36" s="0"/>
       <c r="AMJ36" s="0"/>
     </row>
-    <row r="37" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="10"/>
+      <c r="B37" s="10"/>
       <c r="C37" s="10"/>
+      <c r="D37" s="10"/>
       <c r="E37" s="7"/>
       <c r="F37" s="8"/>
       <c r="G37" s="9"/>
+      <c r="H37" s="10"/>
       <c r="I37" s="0"/>
       <c r="J37" s="0"/>
       <c r="K37" s="0"/>
@@ -38586,11 +38663,15 @@
       <c r="AMI37" s="0"/>
       <c r="AMJ37" s="0"/>
     </row>
-    <row r="38" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="10"/>
+      <c r="B38" s="10"/>
       <c r="C38" s="10"/>
+      <c r="D38" s="10"/>
       <c r="E38" s="7"/>
       <c r="F38" s="8"/>
       <c r="G38" s="9"/>
+      <c r="H38" s="10"/>
       <c r="I38" s="0"/>
       <c r="J38" s="0"/>
       <c r="K38" s="0"/>
@@ -39608,11 +39689,15 @@
       <c r="AMI38" s="0"/>
       <c r="AMJ38" s="0"/>
     </row>
-    <row r="39" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="10"/>
+      <c r="B39" s="10"/>
       <c r="C39" s="10"/>
+      <c r="D39" s="10"/>
       <c r="E39" s="7"/>
       <c r="F39" s="8"/>
       <c r="G39" s="9"/>
+      <c r="H39" s="10"/>
       <c r="I39" s="0"/>
       <c r="J39" s="0"/>
       <c r="K39" s="0"/>
@@ -40630,11 +40715,15 @@
       <c r="AMI39" s="0"/>
       <c r="AMJ39" s="0"/>
     </row>
-    <row r="40" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="10"/>
+      <c r="B40" s="10"/>
       <c r="C40" s="10"/>
+      <c r="D40" s="10"/>
       <c r="E40" s="7"/>
       <c r="F40" s="8"/>
       <c r="G40" s="9"/>
+      <c r="H40" s="10"/>
       <c r="I40" s="0"/>
       <c r="J40" s="0"/>
       <c r="K40" s="0"/>
@@ -41652,11 +41741,15 @@
       <c r="AMI40" s="0"/>
       <c r="AMJ40" s="0"/>
     </row>
-    <row r="41" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="10"/>
+      <c r="B41" s="10"/>
       <c r="C41" s="10"/>
+      <c r="D41" s="10"/>
       <c r="E41" s="7"/>
       <c r="F41" s="8"/>
       <c r="G41" s="9"/>
+      <c r="H41" s="10"/>
       <c r="I41" s="0"/>
       <c r="J41" s="0"/>
       <c r="K41" s="0"/>
@@ -42674,11 +42767,15 @@
       <c r="AMI41" s="0"/>
       <c r="AMJ41" s="0"/>
     </row>
-    <row r="42" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="10"/>
+      <c r="B42" s="10"/>
       <c r="C42" s="10"/>
+      <c r="D42" s="10"/>
       <c r="E42" s="7"/>
       <c r="F42" s="8"/>
       <c r="G42" s="9"/>
+      <c r="H42" s="10"/>
       <c r="I42" s="0"/>
       <c r="J42" s="0"/>
       <c r="K42" s="0"/>
@@ -43696,11 +43793,15 @@
       <c r="AMI42" s="0"/>
       <c r="AMJ42" s="0"/>
     </row>
-    <row r="43" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="10"/>
+      <c r="B43" s="10"/>
       <c r="C43" s="10"/>
+      <c r="D43" s="10"/>
       <c r="E43" s="7"/>
       <c r="F43" s="8"/>
       <c r="G43" s="9"/>
+      <c r="H43" s="10"/>
       <c r="I43" s="0"/>
       <c r="J43" s="0"/>
       <c r="K43" s="0"/>
@@ -44718,11 +44819,15 @@
       <c r="AMI43" s="0"/>
       <c r="AMJ43" s="0"/>
     </row>
-    <row r="44" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="10"/>
+      <c r="B44" s="10"/>
       <c r="C44" s="10"/>
+      <c r="D44" s="10"/>
       <c r="E44" s="7"/>
       <c r="F44" s="8"/>
       <c r="G44" s="9"/>
+      <c r="H44" s="10"/>
       <c r="I44" s="0"/>
       <c r="J44" s="0"/>
       <c r="K44" s="0"/>
@@ -45740,11 +45845,15 @@
       <c r="AMI44" s="0"/>
       <c r="AMJ44" s="0"/>
     </row>
-    <row r="45" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="10"/>
+      <c r="B45" s="10"/>
       <c r="C45" s="10"/>
+      <c r="D45" s="10"/>
       <c r="E45" s="7"/>
       <c r="F45" s="8"/>
       <c r="G45" s="9"/>
+      <c r="H45" s="10"/>
       <c r="I45" s="0"/>
       <c r="J45" s="0"/>
       <c r="K45" s="0"/>
@@ -46762,11 +46871,15 @@
       <c r="AMI45" s="0"/>
       <c r="AMJ45" s="0"/>
     </row>
-    <row r="46" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="10"/>
+      <c r="B46" s="10"/>
       <c r="C46" s="10"/>
+      <c r="D46" s="10"/>
       <c r="E46" s="7"/>
       <c r="F46" s="8"/>
       <c r="G46" s="9"/>
+      <c r="H46" s="10"/>
       <c r="I46" s="0"/>
       <c r="J46" s="0"/>
       <c r="K46" s="0"/>
@@ -47784,11 +47897,15 @@
       <c r="AMI46" s="0"/>
       <c r="AMJ46" s="0"/>
     </row>
-    <row r="47" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="10"/>
+      <c r="B47" s="10"/>
       <c r="C47" s="10"/>
+      <c r="D47" s="10"/>
       <c r="E47" s="7"/>
       <c r="F47" s="8"/>
       <c r="G47" s="9"/>
+      <c r="H47" s="10"/>
       <c r="I47" s="0"/>
       <c r="J47" s="0"/>
       <c r="K47" s="0"/>
@@ -48806,11 +48923,15 @@
       <c r="AMI47" s="0"/>
       <c r="AMJ47" s="0"/>
     </row>
-    <row r="48" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="10"/>
+      <c r="B48" s="10"/>
       <c r="C48" s="10"/>
+      <c r="D48" s="10"/>
       <c r="E48" s="7"/>
       <c r="F48" s="8"/>
       <c r="G48" s="9"/>
+      <c r="H48" s="10"/>
       <c r="I48" s="0"/>
       <c r="J48" s="0"/>
       <c r="K48" s="0"/>
@@ -49828,7 +49949,7 @@
       <c r="AMI48" s="0"/>
       <c r="AMJ48" s="0"/>
     </row>
-    <row r="49" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
         <v>8</v>
       </c>
@@ -50993,13 +51114,16 @@
   <dimension ref="D4:F13"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E15" activeCellId="1" sqref="4:4 E15"/>
+      <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="A:H"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.9132653061224"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.2397959183673"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
11257 - altera arquivo para testes
</commit_message>
<xml_diff>
--- a/src/test/resources/arquivo_usuario/planilha.xlsx
+++ b/src/test/resources/arquivo_usuario/planilha.xlsx
@@ -155,7 +155,7 @@
     <t xml:space="preserve">ANALICE DA CONCEICAO</t>
   </si>
   <si>
-    <t xml:space="preserve">n.analice.conceica.com.br</t>
+    <t xml:space="preserve">ADMIN@XBRAIN.COM.BR</t>
   </si>
   <si>
     <t xml:space="preserve">AGENTE AUTORIZADO NACIONAL</t>
@@ -450,17 +450,17 @@
   </sheetPr>
   <dimension ref="1:49"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="A:H"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E19" activeCellId="0" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="8" min="1" style="1" width="36.1224489795918"/>
-    <col collapsed="false" hidden="false" max="14" min="9" style="2" width="6.88265306122449"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="2" width="18.2244897959184"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="2" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="1025" min="17" style="2" width="6.88265306122449"/>
+    <col collapsed="false" hidden="false" max="8" min="1" style="1" width="35.6377551020408"/>
+    <col collapsed="false" hidden="false" max="14" min="9" style="2" width="6.75"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="2" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="2" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="1025" min="17" style="2" width="6.75"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -19151,7 +19151,7 @@
         <v>38</v>
       </c>
       <c r="E19" s="7" t="n">
-        <v>6920673452</v>
+        <v>28667582506</v>
       </c>
       <c r="F19" s="8" t="s">
         <v>39</v>
@@ -51096,6 +51096,9 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="F49" r:id="rId1" display="ADMIN@XBRAIN.COM.BR"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.511805555555555" right="0.511805555555555" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -51114,16 +51117,16 @@
   <dimension ref="D4:F13"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="A:H"/>
+      <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.2397959183673"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.8316326530612"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
11518 - edita arquivo
</commit_message>
<xml_diff>
--- a/src/test/resources/arquivo_usuario/planilha.xlsx
+++ b/src/test/resources/arquivo_usuario/planilha.xlsx
@@ -56,7 +56,7 @@
     <t xml:space="preserve">VENDEDOR</t>
   </si>
   <si>
-    <t xml:space="preserve">AGENTE_AUTORIZADO</t>
+    <t xml:space="preserve">fghfghf</t>
   </si>
   <si>
     <t xml:space="preserve">ADAIDE SAMANTA DA SILVA SANTOS</t>
@@ -451,16 +451,16 @@
   <dimension ref="1:49"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E19" activeCellId="0" sqref="E19"/>
+      <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="8" min="1" style="1" width="35.6377551020408"/>
-    <col collapsed="false" hidden="false" max="14" min="9" style="2" width="6.75"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="2" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="2" width="9.58673469387755"/>
-    <col collapsed="false" hidden="false" max="1025" min="17" style="2" width="6.75"/>
+    <col collapsed="false" hidden="false" max="8" min="1" style="1" width="35.0969387755102"/>
+    <col collapsed="false" hidden="false" max="14" min="9" style="2" width="6.61224489795918"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="2" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="2" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="1025" min="17" style="2" width="6.61224489795918"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -51122,11 +51122,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.8316326530612"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.4285714285714"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.10204081632653"/>
   </cols>
   <sheetData>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
#12802 - Refatora codigo e corrige testes
</commit_message>
<xml_diff>
--- a/src/test/resources/arquivo_usuario/planilha.xlsx
+++ b/src/test/resources/arquivo_usuario/planilha.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="CRIAÇÃO DE USUARIO CONEXAO" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="62">
   <si>
     <t xml:space="preserve">NIVEL/CANAL</t>
   </si>
@@ -53,7 +53,7 @@
     <t xml:space="preserve">RECEPTIVO</t>
   </si>
   <si>
-    <t xml:space="preserve">VENDEDOR</t>
+    <t xml:space="preserve">               VENDEDOR RECEPTIVO</t>
   </si>
   <si>
     <t xml:space="preserve">AGENTE_AUTORIZADO</t>
@@ -65,7 +65,13 @@
     <t xml:space="preserve">n.adaide.santos@aec.com.br</t>
   </si>
   <si>
+    <t xml:space="preserve">(51) 3322-1010</t>
+  </si>
+  <si>
     <t xml:space="preserve">AGENTE AUTORIZADO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VENDEDOR</t>
   </si>
   <si>
     <t xml:space="preserve">COMERCIAL</t>
@@ -80,10 +86,16 @@
     <t xml:space="preserve">RECEPTIVA</t>
   </si>
   <si>
+    <t xml:space="preserve">VENDEDOR RECEPTIVO</t>
+  </si>
+  <si>
     <t xml:space="preserve">ADRIANA DE LIMA BEZERRA</t>
   </si>
   <si>
     <t xml:space="preserve">n.adriana.lbezerra@aec.com.br</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VENDEDOR RECEPTIVO                </t>
   </si>
   <si>
     <t xml:space="preserve">ALAN DAVISON BARROS SILVA</t>
@@ -102,6 +114,9 @@
   </si>
   <si>
     <t xml:space="preserve">n.amanda.gouveia@aec.com.br</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(51) 99810-8030</t>
   </si>
   <si>
     <t xml:space="preserve">AMANDA CAROLINA DE OLIVEIRA ANDRADE</t>
@@ -125,6 +140,9 @@
     <t xml:space="preserve">ANA CRISTINA FERREIRA DE MEDEIROS</t>
   </si>
   <si>
+    <t xml:space="preserve">101.440.347-27</t>
+  </si>
+  <si>
     <t xml:space="preserve">n.ana.fmedeiros@aec.com.br</t>
   </si>
   <si>
@@ -137,10 +155,16 @@
     <t xml:space="preserve">ANA KAROLINE DA COSTA SANTOS</t>
   </si>
   <si>
+    <t xml:space="preserve">700.289.864-74</t>
+  </si>
+  <si>
     <t xml:space="preserve">n.ana.csantos@aec.com.br</t>
   </si>
   <si>
     <t xml:space="preserve">ANA PAULA BARBOSA TOMAZ SANTOS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">286.675.825-06</t>
   </si>
   <si>
     <t xml:space="preserve">n.ana.tsantos@aec.com.br</t>
@@ -448,19 +472,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:49"/>
+  <dimension ref="A1:AMJ49"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="2:3"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H8" activeCellId="0" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="8" min="1" style="1" width="33.8826530612245"/>
-    <col collapsed="false" hidden="false" max="14" min="9" style="2" width="6.20918367346939"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="2" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="2" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="1025" min="17" style="2" width="6.20918367346939"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="1" style="1" width="33.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="9" style="2" width="6.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="2" width="17.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="2" width="9.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="17" style="2" width="6.21"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1527,8 +1551,8 @@
       <c r="G2" s="9" t="n">
         <v>34218</v>
       </c>
-      <c r="H2" s="1" t="n">
-        <v>51991301817</v>
+      <c r="H2" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="I2" s="0"/>
       <c r="J2" s="0"/>
@@ -2549,20 +2573,20 @@
     </row>
     <row r="3" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E3" s="7"/>
       <c r="F3" s="8" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="G3" s="9" t="n">
         <v>31944</v>
@@ -3589,22 +3613,22 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E4" s="7" t="n">
         <v>70159931479</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="G4" s="9" t="n">
         <v>34436</v>
@@ -4634,19 +4658,19 @@
         <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="E5" s="7" t="n">
         <v>2917600403</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="G5" s="9" t="n">
         <v>27678</v>
@@ -5676,19 +5700,19 @@
         <v>8</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="E6" s="7" t="n">
         <v>9249138431</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="G6" s="9" t="n">
         <v>32373</v>
@@ -6718,25 +6742,25 @@
         <v>8</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="E7" s="7" t="n">
         <v>12532343451</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="G7" s="9" t="n">
         <v>35926</v>
       </c>
-      <c r="H7" s="1" t="n">
-        <v>51991301817</v>
+      <c r="H7" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="I7" s="0"/>
       <c r="J7" s="0"/>
@@ -7760,19 +7784,19 @@
         <v>8</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="E8" s="7" t="n">
         <v>11523845465</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="G8" s="9" t="n">
         <v>34705</v>
@@ -8802,19 +8826,19 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="E9" s="7" t="n">
         <v>1581072414</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="G9" s="9" t="n">
         <v>32575</v>
@@ -9844,19 +9868,19 @@
         <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="E10" s="7" t="n">
         <v>10161857400</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="G10" s="9" t="n">
         <v>33127</v>
@@ -16016,19 +16040,19 @@
         <v>8</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
-      <c r="E16" s="7" t="n">
-        <v>10144034727</v>
+      <c r="E16" s="7" t="s">
+        <v>38</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="G16" s="9" t="n">
         <v>31722</v>
@@ -17058,19 +17082,19 @@
         <v>8</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="E17" s="7" t="n">
         <v>5985368416</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="G17" s="9" t="n">
         <v>31827</v>
@@ -18100,19 +18124,19 @@
         <v>8</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
-      <c r="E18" s="7" t="n">
-        <v>70028986474</v>
+      <c r="E18" s="7" t="s">
+        <v>43</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="G18" s="9" t="n">
         <v>34532</v>
@@ -19142,19 +19166,19 @@
         <v>8</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
-      <c r="E19" s="7" t="n">
-        <v>28667582506</v>
+      <c r="E19" s="7" t="s">
+        <v>46</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="G19" s="9" t="n">
         <v>31751</v>
@@ -20184,19 +20208,19 @@
         <v>8</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="E20" s="7" t="n">
         <v>2131</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="G20" s="9" t="n">
         <v>30749</v>
@@ -49954,19 +49978,19 @@
         <v>8</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="E49" s="7" t="n">
         <v>9460873421</v>
       </c>
       <c r="F49" s="8" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="G49" s="9" t="n">
         <v>34055</v>
@@ -51101,7 +51125,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.511805555555555" right="0.511805555555555" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -51116,58 +51140,58 @@
   </sheetPr>
   <dimension ref="D4:F13"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E15" activeCellId="1" sqref="2:3 E15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.2142857142857"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.36734693877551"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="0" width="8.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="28.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="8.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="9.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="8.37"/>
   </cols>
   <sheetData>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D4" s="0" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D5" s="0" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D6" s="0" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D7" s="0" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D8" s="0" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D9" s="0" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D10" s="0" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -51177,18 +51201,18 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D12" s="0" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D13" s="0" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.511805555555555" right="0.511805555555555" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
#12802 - Aplica code review
</commit_message>
<xml_diff>
--- a/src/test/resources/arquivo_usuario/planilha.xlsx
+++ b/src/test/resources/arquivo_usuario/planilha.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="61">
   <si>
     <t xml:space="preserve">NIVEL/CANAL</t>
   </si>
@@ -81,9 +81,6 @@
   </si>
   <si>
     <t xml:space="preserve">n.adenildo.oliveira@aec.com.br</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RECEPTIVA</t>
   </si>
   <si>
     <t xml:space="preserve">VENDEDOR RECEPTIVO</t>
@@ -474,8 +471,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ49"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H8" activeCellId="0" sqref="H8"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3613,22 +3610,22 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E4" s="7" t="n">
         <v>70159931479</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G4" s="9" t="n">
         <v>34436</v>
@@ -4658,19 +4655,19 @@
         <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E5" s="7" t="n">
         <v>2917600403</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G5" s="9" t="n">
         <v>27678</v>
@@ -5700,19 +5697,19 @@
         <v>8</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E6" s="7" t="n">
         <v>9249138431</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G6" s="9" t="n">
         <v>32373</v>
@@ -6742,25 +6739,25 @@
         <v>8</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E7" s="7" t="n">
         <v>12532343451</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G7" s="9" t="n">
         <v>35926</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I7" s="0"/>
       <c r="J7" s="0"/>
@@ -7784,19 +7781,19 @@
         <v>8</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E8" s="7" t="n">
         <v>11523845465</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G8" s="9" t="n">
         <v>34705</v>
@@ -8826,19 +8823,19 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E9" s="7" t="n">
         <v>1581072414</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G9" s="9" t="n">
         <v>32575</v>
@@ -9868,19 +9865,19 @@
         <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E10" s="7" t="n">
         <v>10161857400</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G10" s="9" t="n">
         <v>33127</v>
@@ -16040,19 +16037,19 @@
         <v>8</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D16" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E16" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="E16" s="7" t="s">
+      <c r="F16" s="8" t="s">
         <v>38</v>
-      </c>
-      <c r="F16" s="8" t="s">
-        <v>39</v>
       </c>
       <c r="G16" s="9" t="n">
         <v>31722</v>
@@ -17082,19 +17079,19 @@
         <v>8</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E17" s="7" t="n">
         <v>5985368416</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G17" s="9" t="n">
         <v>31827</v>
@@ -18124,19 +18121,19 @@
         <v>8</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D18" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E18" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="E18" s="7" t="s">
+      <c r="F18" s="8" t="s">
         <v>43</v>
-      </c>
-      <c r="F18" s="8" t="s">
-        <v>44</v>
       </c>
       <c r="G18" s="9" t="n">
         <v>34532</v>
@@ -19166,19 +19163,19 @@
         <v>8</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D19" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E19" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="E19" s="7" t="s">
+      <c r="F19" s="8" t="s">
         <v>46</v>
-      </c>
-      <c r="F19" s="8" t="s">
-        <v>47</v>
       </c>
       <c r="G19" s="9" t="n">
         <v>31751</v>
@@ -20208,19 +20205,19 @@
         <v>8</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E20" s="7" t="n">
         <v>2131</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G20" s="9" t="n">
         <v>30749</v>
@@ -49984,13 +49981,13 @@
         <v>16</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E49" s="7" t="n">
         <v>9460873421</v>
       </c>
       <c r="F49" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G49" s="9" t="n">
         <v>34055</v>
@@ -51155,7 +51152,7 @@
   <sheetData>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D4" s="0" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F4" s="0" t="s">
         <v>15</v>
@@ -51163,35 +51160,35 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D5" s="0" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D6" s="0" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D7" s="0" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D8" s="0" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D9" s="0" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D10" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -51201,12 +51198,12 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D12" s="0" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D13" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>